<commit_message>
Inicio de presupuesto de 13 mil
</commit_message>
<xml_diff>
--- a/Counts_V3.xlsx
+++ b/Counts_V3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josuez-c\Documents\Personal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josuez-c\Desktop\Personal\Udemy\Git\Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E55EDD-5D10-46D9-9296-2F5D8B4682DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E84BC7-36A2-416B-B3D7-AC847BBEAF0A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="14" activeTab="14" xr2:uid="{608168D3-9D0A-4B9A-96DD-5CA579F2C99B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="11" activeTab="12" xr2:uid="{608168D3-9D0A-4B9A-96DD-5CA579F2C99B}"/>
   </bookViews>
   <sheets>
     <sheet name="15 Feb" sheetId="3" r:id="rId1"/>
@@ -45,6 +45,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -146,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="115">
   <si>
     <t>Concepto</t>
   </si>
@@ -3175,7 +3176,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B7BCF11-46FD-47D8-B733-2158216C0325}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -3231,10 +3232,13 @@
         <v>8</v>
       </c>
       <c r="E3">
-        <v>1800</v>
+        <v>1795</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
+      </c>
+      <c r="H3">
+        <v>2000</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -3242,13 +3246,10 @@
         <v>28</v>
       </c>
       <c r="B4">
-        <v>1450</v>
+        <v>1440</v>
       </c>
       <c r="G4" t="s">
         <v>13</v>
-      </c>
-      <c r="H4">
-        <v>300</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3256,16 +3257,19 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>4900</v>
+        <v>8415</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
       </c>
-      <c r="H5">
-        <v>600</v>
-      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>500</v>
+      </c>
       <c r="G6" t="s">
         <v>15</v>
       </c>
@@ -3292,14 +3296,11 @@
       </c>
       <c r="E9">
         <f>SUM(E3:E8)</f>
-        <v>1800</v>
+        <v>1795</v>
       </c>
       <c r="G9" t="s">
         <v>73</v>
       </c>
-      <c r="H9">
-        <v>1000</v>
-      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -3307,14 +3308,14 @@
       </c>
       <c r="B10">
         <f>SUM(B3:B9)</f>
-        <v>7200</v>
+        <v>11205</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
       </c>
       <c r="H10">
         <f>SUM(H3:H9)</f>
-        <v>4000</v>
+        <v>4100</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -3340,20 +3341,28 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>15000</v>
+        <v>13000</v>
       </c>
       <c r="E18" s="5">
         <f>B23-B10-H10-E9</f>
         <v>2000</v>
       </c>
     </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19">
+        <v>6100</v>
+      </c>
+    </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
       <c r="B23">
         <f>SUM(B18:B22)</f>
-        <v>15000</v>
+        <v>19100</v>
       </c>
     </row>
   </sheetData>
@@ -3434,6 +3443,9 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
+      <c r="E3">
+        <v>2000</v>
+      </c>
       <c r="G3" t="s">
         <v>11</v>
       </c>
@@ -3451,25 +3463,25 @@
       <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="H4">
-        <v>300</v>
-      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5">
-        <v>4900</v>
+        <v>7000</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
       </c>
-      <c r="H5">
-        <v>500</v>
-      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>700</v>
+      </c>
       <c r="G6" t="s">
         <v>15</v>
       </c>
@@ -3496,14 +3508,11 @@
       </c>
       <c r="E9">
         <f>SUM(E3:E8)</f>
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="G9" t="s">
         <v>73</v>
       </c>
-      <c r="H9">
-        <v>1000</v>
-      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -3511,14 +3520,14 @@
       </c>
       <c r="B10">
         <f>SUM(B3:B9)</f>
-        <v>7200</v>
+        <v>10000</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
       </c>
       <c r="H10">
         <f>SUM(H3:H9)</f>
-        <v>5900</v>
+        <v>4100</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -3561,11 +3570,11 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>15000</v>
+        <v>13000</v>
       </c>
       <c r="E18" s="13">
         <f>B23-B10-H10-E9</f>
-        <v>1900</v>
+        <v>2000</v>
       </c>
       <c r="H18">
         <v>7000</v>
@@ -3575,13 +3584,21 @@
         <v>9639.3442622950824</v>
       </c>
     </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19">
+        <v>5100</v>
+      </c>
+    </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
       <c r="B23">
         <f>SUM(B18:B22)</f>
-        <v>15000</v>
+        <v>18100</v>
       </c>
     </row>
   </sheetData>
@@ -3608,7 +3625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F58B53A3-E8D1-4AF7-B935-314F83946148}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Archivo antes de prestamos 15K
</commit_message>
<xml_diff>
--- a/Counts_V3.xlsx
+++ b/Counts_V3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josuez-c\Desktop\Personal\Udemy\Git\Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E84BC7-36A2-416B-B3D7-AC847BBEAF0A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F876C6E-EC94-4E69-A615-9A9FE1312CED}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="11" activeTab="12" xr2:uid="{608168D3-9D0A-4B9A-96DD-5CA579F2C99B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="12" activeTab="13" xr2:uid="{608168D3-9D0A-4B9A-96DD-5CA579F2C99B}"/>
   </bookViews>
   <sheets>
     <sheet name="15 Feb" sheetId="3" r:id="rId1"/>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="114">
   <si>
     <t>Concepto</t>
   </si>
@@ -477,9 +477,6 @@
   </si>
   <si>
     <t>Monto a pagar (Aprox)</t>
-  </si>
-  <si>
-    <t>Zero/Free</t>
   </si>
   <si>
     <t>Samborns/Banorte</t>
@@ -2844,7 +2841,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G8" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H8">
         <v>1500</v>
@@ -2945,7 +2942,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3053,7 +3050,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B7" s="6">
         <v>300</v>
@@ -3067,7 +3064,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B8" s="6">
         <v>500</v>
@@ -3176,7 +3173,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B7BCF11-46FD-47D8-B733-2158216C0325}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -3225,19 +3222,19 @@
       <c r="A3" t="s">
         <v>44</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="6">
         <v>850</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E3">
-        <v>1795</v>
+      <c r="E3" s="6">
+        <v>1600</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="6">
         <v>2000</v>
       </c>
     </row>
@@ -3245,7 +3242,7 @@
       <c r="A4" t="s">
         <v>28</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="6">
         <v>1440</v>
       </c>
       <c r="G4" t="s">
@@ -3256,7 +3253,7 @@
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="6">
         <v>8415</v>
       </c>
       <c r="G5" t="s">
@@ -3267,21 +3264,21 @@
       <c r="A6" t="s">
         <v>20</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="6">
         <v>500</v>
       </c>
       <c r="G6" t="s">
         <v>15</v>
       </c>
-      <c r="H6">
-        <v>1500</v>
+      <c r="H6" s="6">
+        <v>1700</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G7" t="s">
         <v>24</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="6">
         <v>600</v>
       </c>
     </row>
@@ -3296,7 +3293,7 @@
       </c>
       <c r="E9">
         <f>SUM(E3:E8)</f>
-        <v>1795</v>
+        <v>1600</v>
       </c>
       <c r="G9" t="s">
         <v>73</v>
@@ -3315,7 +3312,7 @@
       </c>
       <c r="H10">
         <f>SUM(H3:H9)</f>
-        <v>4100</v>
+        <v>4300</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -3345,7 +3342,7 @@
       </c>
       <c r="E18" s="5">
         <f>B23-B10-H10-E9</f>
-        <v>2000</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -3387,7 +3384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D62384EF-D9B2-497E-AA08-6F8BC70A67AB}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -3444,7 +3441,7 @@
         <v>8</v>
       </c>
       <c r="E3">
-        <v>2000</v>
+        <v>400</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -3469,7 +3466,7 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>7000</v>
+        <v>2000</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
@@ -3486,7 +3483,7 @@
         <v>15</v>
       </c>
       <c r="H6">
-        <v>1500</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -3494,7 +3491,7 @@
         <v>24</v>
       </c>
       <c r="H7">
-        <v>600</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3508,7 +3505,7 @@
       </c>
       <c r="E9">
         <f>SUM(E3:E8)</f>
-        <v>2000</v>
+        <v>400</v>
       </c>
       <c r="G9" t="s">
         <v>73</v>
@@ -3520,14 +3517,14 @@
       </c>
       <c r="B10">
         <f>SUM(B3:B9)</f>
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
       </c>
       <c r="H10">
         <f>SUM(H3:H9)</f>
-        <v>4100</v>
+        <v>5600</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -3577,20 +3574,17 @@
         <v>2000</v>
       </c>
       <c r="H18">
-        <v>7000</v>
+        <v>3400</v>
       </c>
       <c r="I18">
         <f>(H18*I17)/H17</f>
-        <v>9639.3442622950824</v>
+        <v>4681.9672131147545</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
-      <c r="B19">
-        <v>5100</v>
-      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -3598,7 +3592,7 @@
       </c>
       <c r="B23">
         <f>SUM(B18:B22)</f>
-        <v>18100</v>
+        <v>13000</v>
       </c>
     </row>
   </sheetData>
@@ -3682,7 +3676,7 @@
         <v>8</v>
       </c>
       <c r="E3">
-        <v>3600</v>
+        <v>1600</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -3709,9 +3703,6 @@
       <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="B5">
-        <v>1100</v>
-      </c>
       <c r="G5" t="s">
         <v>14</v>
       </c>
@@ -3720,11 +3711,17 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>6000</v>
+      </c>
       <c r="G6" t="s">
         <v>15</v>
       </c>
       <c r="H6">
-        <v>1500</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -3732,7 +3729,7 @@
         <v>24</v>
       </c>
       <c r="H7">
-        <v>600</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3746,14 +3743,11 @@
       </c>
       <c r="E9">
         <f>SUM(E3:E8)</f>
-        <v>3600</v>
+        <v>1600</v>
       </c>
       <c r="G9" t="s">
         <v>73</v>
       </c>
-      <c r="H9">
-        <v>1000</v>
-      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -3761,14 +3755,14 @@
       </c>
       <c r="B10">
         <f>SUM(B3:B9)</f>
-        <v>3400</v>
+        <v>8300</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
       </c>
       <c r="H10">
         <f>SUM(H3:H9)</f>
-        <v>6000</v>
+        <v>6500</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -3806,13 +3800,21 @@
         <v>2000</v>
       </c>
     </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19">
+        <v>3400</v>
+      </c>
+    </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
       <c r="B23">
         <f>SUM(B18:B22)</f>
-        <v>15000</v>
+        <v>18400</v>
       </c>
     </row>
   </sheetData>
@@ -3839,7 +3841,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3891,6 +3893,12 @@
       <c r="B3">
         <v>1450</v>
       </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>950</v>
+      </c>
       <c r="G3" t="s">
         <v>11</v>
       </c>
@@ -3900,10 +3908,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>7</v>
       </c>
       <c r="B4">
-        <v>5550</v>
+        <v>4100</v>
       </c>
       <c r="G4" t="s">
         <v>13</v>
@@ -3925,7 +3933,7 @@
         <v>15</v>
       </c>
       <c r="H6">
-        <v>1500</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -3933,7 +3941,7 @@
         <v>24</v>
       </c>
       <c r="H7">
-        <v>600</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3947,14 +3955,11 @@
       </c>
       <c r="E9">
         <f>SUM(E3:E8)</f>
-        <v>0</v>
+        <v>950</v>
       </c>
       <c r="G9" t="s">
         <v>73</v>
       </c>
-      <c r="H9">
-        <v>1000</v>
-      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -3962,14 +3967,14 @@
       </c>
       <c r="B10">
         <f>SUM(B3:B9)</f>
-        <v>7000</v>
+        <v>5550</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
       </c>
       <c r="H10">
         <f>SUM(H3:H9)</f>
-        <v>6000</v>
+        <v>6500</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -4101,7 +4106,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4">
         <v>5550</v>
@@ -4931,7 +4936,7 @@
       </c>
       <c r="C4">
         <f>Laptop!D17</f>
-        <v>2505</v>
+        <v>1670</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>28</v>
@@ -5057,7 +5062,7 @@
       </c>
       <c r="C13">
         <f>SUM(C3:C12)</f>
-        <v>10810</v>
+        <v>9975</v>
       </c>
     </row>
   </sheetData>
@@ -5234,9 +5239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52DEFC28-569B-4505-9F81-B6FB23EA0CD9}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5394,14 +5397,17 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11">
+      <c r="B11" s="6">
         <v>10</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="6">
         <v>835</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -5441,7 +5447,7 @@
       </c>
       <c r="D17">
         <f>D15-SUMIFS(D2:D13,E2:E13,"1")</f>
-        <v>2505</v>
+        <v>1670</v>
       </c>
     </row>
   </sheetData>
@@ -5457,7 +5463,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="D3" sqref="D3:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Presupuesto para salir de deudas a fin de año, para prestamo 15K y Carro
</commit_message>
<xml_diff>
--- a/Counts_V3.xlsx
+++ b/Counts_V3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josuez-c\Desktop\Personal\Udemy\Git\Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF4D47C-3963-4DA3-B01E-FF84771437D2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C185F79-1A5C-4D76-BB84-2D004B1AB0C5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="12" activeTab="13" xr2:uid="{608168D3-9D0A-4B9A-96DD-5CA579F2C99B}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="13" activeTab="13" xr2:uid="{608168D3-9D0A-4B9A-96DD-5CA579F2C99B}"/>
   </bookViews>
   <sheets>
     <sheet name="15 Feb" sheetId="3" r:id="rId1"/>
@@ -31,11 +31,16 @@
     <sheet name="30 Septiembre" sheetId="24" r:id="rId16"/>
     <sheet name="15 Octubre" sheetId="25" r:id="rId17"/>
     <sheet name="30 Octubre" sheetId="26" r:id="rId18"/>
-    <sheet name="15 Noviembre" sheetId="27" r:id="rId19"/>
-    <sheet name="Deudas" sheetId="6" r:id="rId20"/>
-    <sheet name="Jazz" sheetId="19" r:id="rId21"/>
-    <sheet name="Laptop" sheetId="20" r:id="rId22"/>
-    <sheet name="AT&amp;T" sheetId="21" r:id="rId23"/>
+    <sheet name="15 Noviembre" sheetId="29" r:id="rId19"/>
+    <sheet name="30 Noviembre" sheetId="30" r:id="rId20"/>
+    <sheet name="15 Diciembre" sheetId="32" r:id="rId21"/>
+    <sheet name="30 Diciembre" sheetId="33" r:id="rId22"/>
+    <sheet name="Deudas" sheetId="6" r:id="rId23"/>
+    <sheet name="Jazz 2" sheetId="28" r:id="rId24"/>
+    <sheet name="Laptop" sheetId="20" r:id="rId25"/>
+    <sheet name="AT&amp;T" sheetId="21" r:id="rId26"/>
+    <sheet name="Jazz" sheetId="19" r:id="rId27"/>
+    <sheet name="Neon" sheetId="31" r:id="rId28"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -147,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="121">
   <si>
     <t>Concepto</t>
   </si>
@@ -479,9 +484,6 @@
     <t>Monto a pagar (Aprox)</t>
   </si>
   <si>
-    <t>Samborns/Banorte</t>
-  </si>
-  <si>
     <t>Guadalajara</t>
   </si>
   <si>
@@ -489,6 +491,30 @@
   </si>
   <si>
     <t>Deuda Rafa</t>
+  </si>
+  <si>
+    <t>Auto</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
+  </si>
+  <si>
+    <t>Prestamo 15K</t>
+  </si>
+  <si>
+    <t>Otras Deudas</t>
+  </si>
+  <si>
+    <t>Otras-Deudas</t>
+  </si>
+  <si>
+    <t>Otras-deudas</t>
+  </si>
+  <si>
+    <t>Casa</t>
+  </si>
+  <si>
+    <t>Neon</t>
   </si>
 </sst>
 </file>
@@ -592,7 +618,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -617,6 +643,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -626,7 +655,34 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="58">
+  <dxfs count="67">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -837,6 +893,185 @@
 </file>
 
 <file path=xl/tables/table100.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="105" xr:uid="{BD444082-668C-465E-8E5A-2648EDC88476}" name="Table161014192327313539525762675859196101106" displayName="Table161014192327313539525762675859196101106" ref="A2:B10" totalsRowShown="0">
+  <autoFilter ref="A2:B10" xr:uid="{118E6C9A-65CE-41B2-9CDA-E2E803A2ACA4}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{6CB9F6C8-C941-411B-BA68-51086949A6F0}" name="Concepto"/>
+    <tableColumn id="2" xr3:uid="{CA6B8CE4-F92F-4FD1-B7D7-80157B922C6D}" name="Monto"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table101.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="106" xr:uid="{77629009-D81D-4AC6-AAFD-5A6E426D1416}" name="Table2711152024283236405358636880869297102107" displayName="Table2711152024283236405358636880869297102107" ref="G2:H10" totalsRowShown="0">
+  <autoFilter ref="G2:H10" xr:uid="{55D0E6FB-2E76-4927-9D34-9CAA769EF7F7}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{797D763E-C0DE-4D79-AF56-F9CD00E68FE8}" name="Concepto"/>
+    <tableColumn id="2" xr3:uid="{43A0B299-263A-4157-801F-40D87D34E2D4}" name="Monto"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table102.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="107" xr:uid="{BA84FDCA-BD7E-4196-892D-B3329C234F27}" name="Table712162125293337415459646981879398103108" displayName="Table712162125293337415459646981879398103108" ref="A17:B23" totalsRowShown="0">
+  <autoFilter ref="A17:B23" xr:uid="{5ACFFE3C-8C54-4A57-BCD6-735E5CE8DEA7}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{B99E4110-3259-45B8-848C-54A098843682}" name="Concepto"/>
+    <tableColumn id="2" xr3:uid="{3761B08D-82D0-4937-89BC-92D49C0AB4DF}" name="Monto"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table103.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="108" xr:uid="{4031720E-0F95-4EA7-850B-4816832DE48D}" name="Table813172226303438425560657082889499104109" displayName="Table813172226303438425560657082889499104109" ref="E17:E18" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{AA136418-89BA-4512-8280-2F80F616CFFF}" name="Restante" dataDxfId="6">
+      <calculatedColumnFormula>B23-B10-H10-E9</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table104.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="109" xr:uid="{65772710-F64D-4FB6-BA14-124D521E900F}" name="Table4345464748495156616671838995100105110" displayName="Table4345464748495156616671838995100105110" ref="D2:E9" totalsRowShown="0">
+  <autoFilter ref="D2:E9" xr:uid="{35909676-23EE-45B1-96DF-AD227C9C3285}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{20EBF0DB-ACD9-473F-8CA5-BEEC10B00008}" name="Concepto"/>
+    <tableColumn id="2" xr3:uid="{FE2066D3-440C-4247-B2CD-238D87E5FF0F}" name="Monto"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table105.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="111" xr:uid="{1CFA8894-1C3C-421D-8413-EBEA7B4934DC}" name="Table16101419232731353952576267585919610173112" displayName="Table16101419232731353952576267585919610173112" ref="A2:B10" totalsRowShown="0">
+  <autoFilter ref="A2:B10" xr:uid="{118E6C9A-65CE-41B2-9CDA-E2E803A2ACA4}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{44912649-E43E-48ED-8917-D392096A62C4}" name="Concepto"/>
+    <tableColumn id="2" xr3:uid="{6F519613-0C35-42ED-B49E-93DE0105E893}" name="Monto"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table106.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="112" xr:uid="{7EBAB4EB-5E5A-41F2-B35A-2D97BEB3C845}" name="Table271115202428323640535863688086929710274113" displayName="Table271115202428323640535863688086929710274113" ref="G2:H10" totalsRowShown="0">
+  <autoFilter ref="G2:H10" xr:uid="{55D0E6FB-2E76-4927-9D34-9CAA769EF7F7}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{60989D41-7BB6-48E5-A12D-B8388F3060E0}" name="Concepto"/>
+    <tableColumn id="2" xr3:uid="{52FA1AFE-C6CC-4A87-84CB-62802F9DD0CE}" name="Monto"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table107.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="113" xr:uid="{423080DD-CE5C-480C-BB58-136905C750E2}" name="Table71216212529333741545964698187939810375114" displayName="Table71216212529333741545964698187939810375114" ref="A17:B23" totalsRowShown="0">
+  <autoFilter ref="A17:B23" xr:uid="{5ACFFE3C-8C54-4A57-BCD6-735E5CE8DEA7}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{D40B5449-BE47-4077-BC63-8C4BA29EF00A}" name="Concepto"/>
+    <tableColumn id="2" xr3:uid="{408F9E12-BBAB-46FC-BC70-BFFC091A5DA1}" name="Monto"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table108.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="114" xr:uid="{E34FDC91-9B3B-449A-9349-4982300F405D}" name="Table81317222630343842556065708288949910476115" displayName="Table81317222630343842556065708288949910476115" ref="E17:E18" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{87008DBD-1138-46AC-AEB4-2C20ADBEBD05}" name="Restante" dataDxfId="3">
+      <calculatedColumnFormula>B23-B10-H10-E9</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table109.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="115" xr:uid="{77B1E7DE-A265-482D-8830-C92FA0E9E23F}" name="Table434546474849515661667183899510010590116" displayName="Table434546474849515661667183899510010590116" ref="D2:E9" totalsRowShown="0">
+  <autoFilter ref="D2:E9" xr:uid="{35909676-23EE-45B1-96DF-AD227C9C3285}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{CDD8F792-B0C8-41ED-9960-F6F2A0326FCF}" name="Concepto"/>
+    <tableColumn id="2" xr3:uid="{F9D65851-DEE4-4F7D-B525-0830553B6180}" name="Monto"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{6DDD1893-37F5-4ED0-ADDE-9822BC0F2675}" name="Table71216" displayName="Table71216" ref="A18:B24" totalsRowShown="0">
+  <autoFilter ref="A18:B24" xr:uid="{5ACFFE3C-8C54-4A57-BCD6-735E5CE8DEA7}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{3EC8B9BC-640A-4601-820D-84FDC0E3E4F3}" name="Concepto"/>
+    <tableColumn id="2" xr3:uid="{28F1514C-48EC-4090-B851-07325ACC5509}" name="Monto"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table110.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="116" xr:uid="{1D95C88F-0BBF-49F3-85FE-40AC1BE32AB4}" name="Table161014192327313539525762675859196101106117" displayName="Table161014192327313539525762675859196101106117" ref="A2:B10" totalsRowShown="0">
+  <autoFilter ref="A2:B10" xr:uid="{118E6C9A-65CE-41B2-9CDA-E2E803A2ACA4}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{CF9FF7F5-1C86-46D0-8FAB-7C7D30923F2A}" name="Concepto"/>
+    <tableColumn id="2" xr3:uid="{EEEF9501-7507-4410-8018-7A1C681260F3}" name="Monto"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table111.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="117" xr:uid="{2BD61BFA-F743-4712-A73F-CAAE8DA445E9}" name="Table2711152024283236405358636880869297102107118" displayName="Table2711152024283236405358636880869297102107118" ref="G2:H10" totalsRowShown="0">
+  <autoFilter ref="G2:H10" xr:uid="{55D0E6FB-2E76-4927-9D34-9CAA769EF7F7}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{F4D6087E-8D27-45C7-87ED-128D0C3B1D13}" name="Concepto"/>
+    <tableColumn id="2" xr3:uid="{18C66E0F-D7B7-4C8F-A592-BC575419BB23}" name="Monto"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table112.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="118" xr:uid="{D4A4AE6F-D5A5-41CB-B1B7-E520F7E7A0EA}" name="Table712162125293337415459646981879398103108119" displayName="Table712162125293337415459646981879398103108119" ref="A17:B23" totalsRowShown="0">
+  <autoFilter ref="A17:B23" xr:uid="{5ACFFE3C-8C54-4A57-BCD6-735E5CE8DEA7}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{174F6A0A-57AF-47D3-B6B1-8EB5665C4CED}" name="Concepto"/>
+    <tableColumn id="2" xr3:uid="{B7BB0147-355D-4091-80F0-3E564F5F550F}" name="Monto"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table113.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="119" xr:uid="{47E7B440-9775-4359-A21B-8717CD3589CE}" name="Table813172226303438425560657082889499104109120" displayName="Table813172226303438425560657082889499104109120" ref="E17:E18" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+  <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{6B7F805A-0C9D-4169-8EB3-B8D113010DB4}" name="Restante" dataDxfId="0">
+      <calculatedColumnFormula>B23-B10-H10-E9</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table114.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="120" xr:uid="{E407E054-CDD6-421B-B619-8CE8355F8C8D}" name="Table4345464748495156616671838995100105110121" displayName="Table4345464748495156616671838995100105110121" ref="D2:E9" totalsRowShown="0">
+  <autoFilter ref="D2:E9" xr:uid="{35909676-23EE-45B1-96DF-AD227C9C3285}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{35AAB6F5-14B4-4DE1-B7C1-87D815CA055B}" name="Concepto"/>
+    <tableColumn id="2" xr3:uid="{1DE8C7BF-C550-40A8-8758-C9657E1609CD}" name="Monto"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table115.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{A7428449-465F-4335-8A22-A04831709D07}" name="Table1618" displayName="Table1618" ref="A2:C13" totalsRowShown="0">
   <autoFilter ref="A2:C13" xr:uid="{A4206556-B7C7-4E7D-80ED-F4D40D255729}"/>
   <tableColumns count="3">
@@ -848,7 +1083,47 @@
 </table>
 </file>
 
-<file path=xl/tables/table101.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table116.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="71" xr:uid="{C1E6F83D-8473-4577-9A45-6FA8E84217EA}" name="Table172" displayName="Table172" ref="A1:C9" totalsRowShown="0">
+  <autoFilter ref="A1:C9" xr:uid="{E85945BF-0347-4283-B4FB-329C892B49AD}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{659E1EC5-6CF7-4805-A951-08AC808E2315}" name="Prestamo 15K"/>
+    <tableColumn id="2" xr3:uid="{C7E6EE69-6473-4311-BAE5-E009EBB8AD06}" name="Concepto"/>
+    <tableColumn id="3" xr3:uid="{F19288B6-DCEF-4DE5-A666-C4F13D6B6FBE}" name="Cantidad"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table117.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="77" xr:uid="{45800315-40D0-4619-A718-EF9AD896042B}" name="Table7678" displayName="Table7678" ref="A1:E15" totalsRowShown="0">
+  <autoFilter ref="A1:E15" xr:uid="{3D62BFF4-E1EC-48EF-8175-8365BDEB915E}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{23767DCA-88E3-48BA-BD4F-2DF0D8275442}" name="Prestamo"/>
+    <tableColumn id="2" xr3:uid="{A29C228D-28F6-45BD-A335-4F589E6F26BD}" name="Numero de abono"/>
+    <tableColumn id="3" xr3:uid="{AB09C49F-C030-48EE-9EFC-A76DB1DB1D60}" name="Fecha"/>
+    <tableColumn id="4" xr3:uid="{611C57B0-106E-4205-BFD3-5A36BFE03917}" name="Pago Quincenal"/>
+    <tableColumn id="5" xr3:uid="{655379D6-3833-4B49-B540-EC16870DE68A}" name="Pagado"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table118.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="78" xr:uid="{C37A6D5E-2C67-42BD-A506-B21D8F530A79}" name="Table767879" displayName="Table767879" ref="A1:E15" totalsRowShown="0">
+  <autoFilter ref="A1:E15" xr:uid="{3D62BFF4-E1EC-48EF-8175-8365BDEB915E}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{69DE7F5D-8101-4A1C-9BE6-A14C0DE80276}" name="Prestamo"/>
+    <tableColumn id="2" xr3:uid="{D6FE761B-0EAC-46E6-B522-20BA216A8B35}" name="Numero de abono"/>
+    <tableColumn id="3" xr3:uid="{58802C2C-F52D-4A72-A4C4-385A7E6BB113}" name="Fecha"/>
+    <tableColumn id="4" xr3:uid="{EC99AD48-7E56-403F-9897-87BBF040DA16}" name="Pago Quincenal"/>
+    <tableColumn id="5" xr3:uid="{D38A51EA-9A7C-4D0B-99C1-0080173C4821}" name="Pagado"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table119.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="76" xr:uid="{97221669-6CC7-4845-8A50-42C4FBDBF442}" name="Table76" displayName="Table76" ref="A1:E10" totalsRowShown="0">
   <autoFilter ref="A1:E10" xr:uid="{3D62BFF4-E1EC-48EF-8175-8365BDEB915E}"/>
   <tableColumns count="5">
@@ -862,54 +1137,27 @@
 </table>
 </file>
 
-<file path=xl/tables/table102.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="77" xr:uid="{45800315-40D0-4619-A718-EF9AD896042B}" name="Table7678" displayName="Table7678" ref="A1:E15" totalsRowShown="0">
-  <autoFilter ref="A1:E15" xr:uid="{3D62BFF4-E1EC-48EF-8175-8365BDEB915E}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{23767DCA-88E3-48BA-BD4F-2DF0D8275442}" name="Prestamo"/>
-    <tableColumn id="2" xr3:uid="{A29C228D-28F6-45BD-A335-4F589E6F26BD}" name="Numero de abono"/>
-    <tableColumn id="3" xr3:uid="{AB09C49F-C030-48EE-9EFC-A76DB1DB1D60}" name="Fecha"/>
-    <tableColumn id="4" xr3:uid="{611C57B0-106E-4205-BFD3-5A36BFE03917}" name="Pago Quincenal"/>
-    <tableColumn id="5" xr3:uid="{655379D6-3833-4B49-B540-EC16870DE68A}" name="Pagado"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table103.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="78" xr:uid="{C37A6D5E-2C67-42BD-A506-B21D8F530A79}" name="Table767879" displayName="Table767879" ref="A1:E15" totalsRowShown="0">
-  <autoFilter ref="A1:E15" xr:uid="{3D62BFF4-E1EC-48EF-8175-8365BDEB915E}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{69DE7F5D-8101-4A1C-9BE6-A14C0DE80276}" name="Prestamo"/>
-    <tableColumn id="2" xr3:uid="{D6FE761B-0EAC-46E6-B522-20BA216A8B35}" name="Numero de abono"/>
-    <tableColumn id="3" xr3:uid="{58802C2C-F52D-4A72-A4C4-385A7E6BB113}" name="Fecha"/>
-    <tableColumn id="4" xr3:uid="{EC99AD48-7E56-403F-9897-87BBF040DA16}" name="Pago Quincenal"/>
-    <tableColumn id="5" xr3:uid="{D38A51EA-9A7C-4D0B-99C1-0080173C4821}" name="Pagado"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{6DDD1893-37F5-4ED0-ADDE-9822BC0F2675}" name="Table71216" displayName="Table71216" ref="A18:B24" totalsRowShown="0">
-  <autoFilter ref="A18:B24" xr:uid="{5ACFFE3C-8C54-4A57-BCD6-735E5CE8DEA7}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3EC8B9BC-640A-4601-820D-84FDC0E3E4F3}" name="Concepto"/>
-    <tableColumn id="2" xr3:uid="{28F1514C-48EC-4090-B851-07325ACC5509}" name="Monto"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{6EB74B2F-5FCA-473F-9FAA-3EDF8111D5D5}" name="Table81317" displayName="Table81317" ref="E17:E18" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{6EB74B2F-5FCA-473F-9FAA-3EDF8111D5D5}" name="Table81317" displayName="Table81317" ref="E17:E18" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{CE9482A1-3934-4F51-997A-9EFBA1863710}" name="Restante" dataDxfId="49">
+    <tableColumn id="1" xr3:uid="{CE9482A1-3934-4F51-997A-9EFBA1863710}" name="Restante" dataDxfId="58">
       <calculatedColumnFormula>B24-B9-H9-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table120.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="110" xr:uid="{B28A211B-7C8D-4126-9D65-5F77542B39C1}" name="Table172111" displayName="Table172111" ref="A1:C9" totalsRowShown="0">
+  <autoFilter ref="A1:C9" xr:uid="{EF8E7F14-6CB0-4C4A-8A71-BFA9216C82C2}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{6321227C-6519-47A4-B4B0-42E465540374}" name="Neon"/>
+    <tableColumn id="2" xr3:uid="{2ED343E1-2965-4190-A788-4786C7867212}" name="Fecha"/>
+    <tableColumn id="3" xr3:uid="{3E2B6380-1FA7-4080-B27F-C9EE1AE2F97F}" name="Cantidad"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -969,10 +1217,10 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{C6113CAB-14DB-4CA9-B83E-7B558420A38C}" name="Table8131722" displayName="Table8131722" ref="E17:E18" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{C6113CAB-14DB-4CA9-B83E-7B558420A38C}" name="Table8131722" displayName="Table8131722" ref="E17:E18" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{17B47C4D-B270-4929-9F44-5483826CC1AE}" name="Restante" dataDxfId="46">
+    <tableColumn id="1" xr3:uid="{17B47C4D-B270-4929-9F44-5483826CC1AE}" name="Restante" dataDxfId="55">
       <calculatedColumnFormula>B23-B11-H9-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1047,10 +1295,10 @@
 </file>
 
 <file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{F627F082-294B-4972-9027-409731C849B1}" name="Table813172226" displayName="Table813172226" ref="E17:E18" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{F627F082-294B-4972-9027-409731C849B1}" name="Table813172226" displayName="Table813172226" ref="E17:E18" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{84805B74-C396-407D-B3EF-AA50F3B88793}" name="Restante" dataDxfId="43">
+    <tableColumn id="1" xr3:uid="{84805B74-C396-407D-B3EF-AA50F3B88793}" name="Restante" dataDxfId="52">
       <calculatedColumnFormula>B23-B11-H9-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1103,10 +1351,10 @@
 </file>
 
 <file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{F2237E1E-DB59-4357-9ED1-E146B786B6E8}" name="Table81317222630" displayName="Table81317222630" ref="E17:E18" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{F2237E1E-DB59-4357-9ED1-E146B786B6E8}" name="Table81317222630" displayName="Table81317222630" ref="E17:E18" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{7FE38D7A-746A-4B78-86EA-E6C48DDBB8A0}" name="Restante" dataDxfId="40">
+    <tableColumn id="1" xr3:uid="{7FE38D7A-746A-4B78-86EA-E6C48DDBB8A0}" name="Restante" dataDxfId="49">
       <calculatedColumnFormula>B23-B11-H9-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1170,10 +1418,10 @@
 </file>
 
 <file path=xl/tables/table34.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{B70A0F6A-8050-4DB3-85A2-CB613921E543}" name="Table8131722263034" displayName="Table8131722263034" ref="E17:E18" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{B70A0F6A-8050-4DB3-85A2-CB613921E543}" name="Table8131722263034" displayName="Table8131722263034" ref="E17:E18" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{291FFC4C-53BF-4611-8650-189C4CE99ED2}" name="Restante" dataDxfId="37">
+    <tableColumn id="1" xr3:uid="{291FFC4C-53BF-4611-8650-189C4CE99ED2}" name="Restante" dataDxfId="46">
       <calculatedColumnFormula>B23-B11-H9-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1226,10 +1474,10 @@
 </file>
 
 <file path=xl/tables/table39.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="37" xr:uid="{6CE768FB-536E-4602-8FA1-80E57812D3D7}" name="Table813172226303438" displayName="Table813172226303438" ref="E17:E18" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="37" xr:uid="{6CE768FB-536E-4602-8FA1-80E57812D3D7}" name="Table813172226303438" displayName="Table813172226303438" ref="E17:E18" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{6A83FD00-1A49-4187-B78E-59E702BF0D8C}" name="Restante" dataDxfId="34">
+    <tableColumn id="1" xr3:uid="{6A83FD00-1A49-4187-B78E-59E702BF0D8C}" name="Restante" dataDxfId="43">
       <calculatedColumnFormula>B23-B11-H9-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1238,10 +1486,10 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{CF7189AF-8506-457B-AF02-678238446516}" name="Table8" displayName="Table8" ref="F14:F15" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{CF7189AF-8506-457B-AF02-678238446516}" name="Table8" displayName="Table8" ref="F14:F15" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
   <autoFilter ref="F14:F15" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{4A560B8E-4A45-4A34-80BB-77B5C3912F5F}" name="Restante" dataDxfId="55">
+    <tableColumn id="1" xr3:uid="{4A560B8E-4A45-4A34-80BB-77B5C3912F5F}" name="Restante" dataDxfId="64">
       <calculatedColumnFormula>B21-B10-F10</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1294,10 +1542,10 @@
 </file>
 
 <file path=xl/tables/table44.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="41" xr:uid="{221D2EBC-F3BE-4FFD-BA8C-2A7B2D5F1F06}" name="Table81317222630343842" displayName="Table81317222630343842" ref="E17:E18" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="41" xr:uid="{221D2EBC-F3BE-4FFD-BA8C-2A7B2D5F1F06}" name="Table81317222630343842" displayName="Table81317222630343842" ref="E17:E18" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{C983AC74-910C-462A-A5AC-E4E7D8251DD7}" name="Restante" dataDxfId="31">
+    <tableColumn id="1" xr3:uid="{C983AC74-910C-462A-A5AC-E4E7D8251DD7}" name="Restante" dataDxfId="40">
       <calculatedColumnFormula>B23-B10-H9-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1394,10 +1642,10 @@
 </file>
 
 <file path=xl/tables/table52.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="54" xr:uid="{D8CF4A15-7D2D-43A1-BDCD-6886F425BACE}" name="Table8131722263034384255" displayName="Table8131722263034384255" ref="E17:E18" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="54" xr:uid="{D8CF4A15-7D2D-43A1-BDCD-6886F425BACE}" name="Table8131722263034384255" displayName="Table8131722263034384255" ref="E17:E18" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{01FC21D7-E33E-4541-80CD-10112E5DAD8E}" name="Restante" dataDxfId="28">
+    <tableColumn id="1" xr3:uid="{01FC21D7-E33E-4541-80CD-10112E5DAD8E}" name="Restante" dataDxfId="37">
       <calculatedColumnFormula>B23-B10-H9-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1450,10 +1698,10 @@
 </file>
 
 <file path=xl/tables/table57.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="59" xr:uid="{78652AD3-F12D-41C4-B189-0D7B21314932}" name="Table813172226303438425560" displayName="Table813172226303438425560" ref="E17:E18" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="59" xr:uid="{78652AD3-F12D-41C4-B189-0D7B21314932}" name="Table813172226303438425560" displayName="Table813172226303438425560" ref="E17:E18" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{3E662EAE-9351-4FAF-8E50-D47E45AE97AC}" name="Restante" dataDxfId="25">
+    <tableColumn id="1" xr3:uid="{3E662EAE-9351-4FAF-8E50-D47E45AE97AC}" name="Restante" dataDxfId="34">
       <calculatedColumnFormula>B23-B10-H9-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1517,10 +1765,10 @@
 </file>
 
 <file path=xl/tables/table62.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="64" xr:uid="{B957AF75-42E6-4BA6-9FC2-1F38625FFD28}" name="Table81317222630343842556065" displayName="Table81317222630343842556065" ref="E17:E18" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="64" xr:uid="{B957AF75-42E6-4BA6-9FC2-1F38625FFD28}" name="Table81317222630343842556065" displayName="Table81317222630343842556065" ref="E17:E18" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{FB468390-A346-49F3-B226-62B380F4E00B}" name="Restante" dataDxfId="22">
+    <tableColumn id="1" xr3:uid="{FB468390-A346-49F3-B226-62B380F4E00B}" name="Restante" dataDxfId="31">
       <calculatedColumnFormula>B23-B10-H10-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1573,10 +1821,10 @@
 </file>
 
 <file path=xl/tables/table67.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="69" xr:uid="{1F763CB0-5D67-4782-B1D1-185995FAF701}" name="Table8131722263034384255606570" displayName="Table8131722263034384255606570" ref="E17:E18" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="69" xr:uid="{1F763CB0-5D67-4782-B1D1-185995FAF701}" name="Table8131722263034384255606570" displayName="Table8131722263034384255606570" ref="E17:E18" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{015756F4-B40A-45B4-A6BD-967346B724AB}" name="Restante" dataDxfId="19">
+    <tableColumn id="1" xr3:uid="{015756F4-B40A-45B4-A6BD-967346B724AB}" name="Restante" dataDxfId="28">
       <calculatedColumnFormula>B23-B10-H10-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1640,10 +1888,10 @@
 </file>
 
 <file path=xl/tables/table72.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="81" xr:uid="{03938C9E-C130-4923-AEFB-4E7EE2A4779E}" name="Table813172226303438425560657082" displayName="Table813172226303438425560657082" ref="E17:E18" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="81" xr:uid="{03938C9E-C130-4923-AEFB-4E7EE2A4779E}" name="Table813172226303438425560657082" displayName="Table813172226303438425560657082" ref="E17:E18" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{36023DA8-4FE9-47DD-B333-A9AFE4EB7204}" name="Restante" dataDxfId="16">
+    <tableColumn id="1" xr3:uid="{36023DA8-4FE9-47DD-B333-A9AFE4EB7204}" name="Restante" dataDxfId="25">
       <calculatedColumnFormula>B23-B10-H10-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1663,7 +1911,7 @@
 </file>
 
 <file path=xl/tables/table74.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="83" xr:uid="{2AF05975-5D9A-45C8-920B-D15CCD6D82B8}" name="Table83" displayName="Table83" ref="H16:I18" totalsRowShown="0" headerRowDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="83" xr:uid="{2AF05975-5D9A-45C8-920B-D15CCD6D82B8}" name="Table83" displayName="Table83" ref="H16:I18" totalsRowShown="0" headerRowDxfId="24">
   <autoFilter ref="H16:I18" xr:uid="{858BF2D4-21A7-4045-A21A-FA9333CB1404}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{98539052-BA4D-4533-AF09-70C6F2D918B6}" name="Monto Pedido"/>
@@ -1709,10 +1957,10 @@
 </file>
 
 <file path=xl/tables/table78.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="87" xr:uid="{E7FB8AF9-F2FC-41D6-A5E7-C62FD5A65876}" name="Table81317222630343842556065708288" displayName="Table81317222630343842556065708288" ref="E17:E18" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="87" xr:uid="{E7FB8AF9-F2FC-41D6-A5E7-C62FD5A65876}" name="Table81317222630343842556065708288" displayName="Table81317222630343842556065708288" ref="E17:E18" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{22311529-0E6B-4E18-B7B7-AABA36467ADA}" name="Restante" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{22311529-0E6B-4E18-B7B7-AABA36467ADA}" name="Restante" dataDxfId="21">
       <calculatedColumnFormula>B23-B10-H10-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1732,10 +1980,10 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{94410419-2417-4F8D-990A-61DB66FE296E}" name="Table813" displayName="Table813" ref="F17:F18" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{94410419-2417-4F8D-990A-61DB66FE296E}" name="Table813" displayName="Table813" ref="F17:F18" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
   <autoFilter ref="F17:F18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{02ABE55D-D08A-4FAB-9216-A7A6F25790A3}" name="Restante" dataDxfId="52">
+    <tableColumn id="1" xr3:uid="{02ABE55D-D08A-4FAB-9216-A7A6F25790A3}" name="Restante" dataDxfId="61">
       <calculatedColumnFormula>B23-C12-F9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1777,10 +2025,10 @@
 </file>
 
 <file path=xl/tables/table83.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="93" xr:uid="{6FA57C93-C1AB-4452-8152-77D321556756}" name="Table8131722263034384255606570828894" displayName="Table8131722263034384255606570828894" ref="E17:E18" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="93" xr:uid="{6FA57C93-C1AB-4452-8152-77D321556756}" name="Table8131722263034384255606570828894" displayName="Table8131722263034384255606570828894" ref="E17:E18" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{823C011F-989F-468A-98EA-B63D69D1F99D}" name="Restante" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{823C011F-989F-468A-98EA-B63D69D1F99D}" name="Restante" dataDxfId="18">
       <calculatedColumnFormula>B23-B10-H10-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1833,10 +2081,10 @@
 </file>
 
 <file path=xl/tables/table88.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="98" xr:uid="{7078DBBC-EA6A-4AED-9677-0F09CF55D199}" name="Table813172226303438425560657082889499" displayName="Table813172226303438425560657082889499" ref="E17:E18" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="98" xr:uid="{7078DBBC-EA6A-4AED-9677-0F09CF55D199}" name="Table813172226303438425560657082889499" displayName="Table813172226303438425560657082889499" ref="E17:E18" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{0F94546F-7898-45CB-A1C2-350CAAC13463}" name="Restante" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{0F94546F-7898-45CB-A1C2-350CAAC13463}" name="Restante" dataDxfId="15">
       <calculatedColumnFormula>B23-B10-H10-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1900,10 +2148,10 @@
 </file>
 
 <file path=xl/tables/table93.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="103" xr:uid="{D51F89B1-71F9-4429-BEFD-E895E05814BA}" name="Table813172226303438425560657082889499104" displayName="Table813172226303438425560657082889499104" ref="E17:E18" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="103" xr:uid="{D51F89B1-71F9-4429-BEFD-E895E05814BA}" name="Table813172226303438425560657082889499104" displayName="Table813172226303438425560657082889499104" ref="E17:E18" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{2D06AE74-1328-4E8B-B2E7-CA17A939DF7F}" name="Restante" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{2D06AE74-1328-4E8B-B2E7-CA17A939DF7F}" name="Restante" dataDxfId="12">
       <calculatedColumnFormula>B23-B10-H10-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1923,43 +2171,43 @@
 </file>
 
 <file path=xl/tables/table95.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="105" xr:uid="{ADF6EFBA-AA5A-4C79-B19D-B8F0242E42FD}" name="Table161014192327313539525762675859196101106" displayName="Table161014192327313539525762675859196101106" ref="A2:B10" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="72" xr:uid="{30ED15C5-06DC-4E44-B521-5DE98839EFD3}" name="Table16101419232731353952576267585919610173" displayName="Table16101419232731353952576267585919610173" ref="A2:B10" totalsRowShown="0">
   <autoFilter ref="A2:B10" xr:uid="{118E6C9A-65CE-41B2-9CDA-E2E803A2ACA4}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{A4FA0F68-BF71-4067-B140-F27B90F42B22}" name="Concepto"/>
-    <tableColumn id="2" xr3:uid="{CD9EEF64-3DF0-4BB2-9E84-674401926A41}" name="Monto"/>
+    <tableColumn id="1" xr3:uid="{60BEA906-FF28-4944-A858-8DF6EE279CB2}" name="Concepto"/>
+    <tableColumn id="2" xr3:uid="{A183BEF3-89BC-4EA4-B3CA-D0CFB828313D}" name="Monto"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table96.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="106" xr:uid="{9C8DBBA6-9F20-4A9F-BC5E-A75E92FC79F0}" name="Table2711152024283236405358636880869297102107" displayName="Table2711152024283236405358636880869297102107" ref="G2:H10" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="73" xr:uid="{B70A5B4A-0D4E-46BB-A3D7-76A6C2CFEC15}" name="Table271115202428323640535863688086929710274" displayName="Table271115202428323640535863688086929710274" ref="G2:H10" totalsRowShown="0">
   <autoFilter ref="G2:H10" xr:uid="{55D0E6FB-2E76-4927-9D34-9CAA769EF7F7}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3D1DFFB2-A009-4594-BA69-BF2EF28FF89F}" name="Concepto"/>
-    <tableColumn id="2" xr3:uid="{28B587F0-60CB-4D6E-B7FA-C82E8D3331EC}" name="Monto"/>
+    <tableColumn id="1" xr3:uid="{ED0A147B-3089-45EB-AB2D-A2E1A16A8163}" name="Concepto"/>
+    <tableColumn id="2" xr3:uid="{0CF9DF16-D6C0-49D9-8B7D-16F4AF278415}" name="Monto"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table97.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="107" xr:uid="{08BB7237-32D3-4BDF-8A6B-A9A8C5650002}" name="Table712162125293337415459646981879398103108" displayName="Table712162125293337415459646981879398103108" ref="A17:B23" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="74" xr:uid="{FFC5D93F-D0F0-439A-BC2B-0FCF618E09DB}" name="Table71216212529333741545964698187939810375" displayName="Table71216212529333741545964698187939810375" ref="A17:B23" totalsRowShown="0">
   <autoFilter ref="A17:B23" xr:uid="{5ACFFE3C-8C54-4A57-BCD6-735E5CE8DEA7}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{44D9BAC0-DF75-491D-8A2D-999A53DE2B9D}" name="Concepto"/>
-    <tableColumn id="2" xr3:uid="{B251A6E3-6A91-4F46-BB50-0DBAC36111BA}" name="Monto"/>
+    <tableColumn id="1" xr3:uid="{42C531B1-C784-4B9D-861C-43BF12994A6E}" name="Concepto"/>
+    <tableColumn id="2" xr3:uid="{43BC3703-F06D-4581-BA97-77A2FCBCC76D}" name="Monto"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table98.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="108" xr:uid="{AD3CCEB1-E354-45E3-B47F-633D9475C54A}" name="Table813172226303438425560657082889499104109" displayName="Table813172226303438425560657082889499104109" ref="E17:E18" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="75" xr:uid="{385F9B9B-E896-4352-A1BA-C6D5B3B94CBD}" name="Table81317222630343842556065708288949910476" displayName="Table81317222630343842556065708288949910476" ref="E17:E18" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{A39615FF-A392-4D07-8E00-5132D1C1E906}" name="Restante" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{0266BF34-9ADC-4818-9E88-FEA6FD539BF6}" name="Restante" dataDxfId="9">
       <calculatedColumnFormula>B23-B10-H10-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1968,11 +2216,11 @@
 </file>
 
 <file path=xl/tables/table99.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="109" xr:uid="{C9532B31-38CF-4102-B8B1-F56FAEEE52BE}" name="Table4345464748495156616671838995100105110" displayName="Table4345464748495156616671838995100105110" ref="D2:E9" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="89" xr:uid="{CB35E77C-BB8D-4BF0-A025-005D8F6CD22E}" name="Table434546474849515661667183899510010590" displayName="Table434546474849515661667183899510010590" ref="D2:E9" totalsRowShown="0">
   <autoFilter ref="D2:E9" xr:uid="{35909676-23EE-45B1-96DF-AD227C9C3285}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{E21673A3-DCF0-42F3-B8B6-8350410FFC3D}" name="Concepto"/>
-    <tableColumn id="2" xr3:uid="{2739CA90-B76A-4552-BC95-53CE79CC42AB}" name="Monto"/>
+    <tableColumn id="1" xr3:uid="{38930260-C22E-447F-BC3C-5F385FDA2E16}" name="Concepto"/>
+    <tableColumn id="2" xr3:uid="{88ACDE1C-DE29-4B11-8592-5C39F1030437}" name="Monto"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2288,14 +2536,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="E1" s="16" t="s">
+      <c r="B1" s="16"/>
+      <c r="E1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="16"/>
+      <c r="F1" s="17"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2399,10 +2647,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="16"/>
+      <c r="B13" s="17"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2502,18 +2750,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="D1" s="16" t="s">
+      <c r="B1" s="16"/>
+      <c r="D1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="G1" s="16" t="s">
+      <c r="E1" s="17"/>
+      <c r="G1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="16"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2651,10 +2899,10 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="16"/>
+      <c r="B16" s="17"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2739,18 +2987,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="D1" s="16" t="s">
+      <c r="B1" s="16"/>
+      <c r="D1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="G1" s="16" t="s">
+      <c r="E1" s="17"/>
+      <c r="G1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="16"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2841,7 +3089,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G8" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H8">
         <v>1500</v>
@@ -2873,10 +3121,10 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="16"/>
+      <c r="B16" s="17"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2953,18 +3201,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="D1" s="16" t="s">
+      <c r="B1" s="16"/>
+      <c r="D1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="G1" s="16" t="s">
+      <c r="E1" s="17"/>
+      <c r="G1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="16"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3050,7 +3298,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B7" s="6">
         <v>300</v>
@@ -3064,7 +3312,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B8" s="6">
         <v>500</v>
@@ -3105,10 +3353,10 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="16"/>
+      <c r="B16" s="17"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3185,18 +3433,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="D1" s="16" t="s">
+      <c r="B1" s="16"/>
+      <c r="D1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="G1" s="16" t="s">
+      <c r="E1" s="17"/>
+      <c r="G1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="16"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3316,10 +3564,10 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="16"/>
+      <c r="B16" s="17"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3397,18 +3645,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="D1" s="16" t="s">
+      <c r="B1" s="16"/>
+      <c r="D1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="G1" s="16" t="s">
+      <c r="E1" s="17"/>
+      <c r="G1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="16"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3437,17 +3685,11 @@
       <c r="B3">
         <v>1450</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <v>400</v>
-      </c>
       <c r="G3" t="s">
         <v>11</v>
       </c>
       <c r="H3">
-        <v>2000</v>
+        <v>7150</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -3460,25 +3702,16 @@
       <c r="G4" t="s">
         <v>13</v>
       </c>
+      <c r="H4">
+        <v>450</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>2000</v>
-      </c>
       <c r="G5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6">
-        <v>700</v>
-      </c>
       <c r="G6" t="s">
         <v>15</v>
       </c>
@@ -3491,7 +3724,7 @@
         <v>24</v>
       </c>
       <c r="H7">
-        <v>1500</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3505,7 +3738,7 @@
       </c>
       <c r="E9">
         <f>SUM(E3:E8)</f>
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="G9" t="s">
         <v>73</v>
@@ -3517,27 +3750,27 @@
       </c>
       <c r="B10">
         <f>SUM(B3:B9)</f>
-        <v>5000</v>
+        <v>2300</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
       </c>
       <c r="H10">
         <f>SUM(H3:H9)</f>
-        <v>5600</v>
+        <v>10700</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H15" s="16" t="s">
+      <c r="H15" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="I15" s="16"/>
+      <c r="I15" s="17"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="16"/>
+      <c r="B16" s="17"/>
       <c r="H16" s="13" t="s">
         <v>108</v>
       </c>
@@ -3567,7 +3800,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>13000</v>
+        <v>15000</v>
       </c>
       <c r="E18" s="13">
         <f>B23-B10-H10-E9</f>
@@ -3581,18 +3814,13 @@
         <v>4681.9672131147545</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>7</v>
-      </c>
-    </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
       <c r="B23">
         <f>SUM(B18:B22)</f>
-        <v>13000</v>
+        <v>15000</v>
       </c>
     </row>
   </sheetData>
@@ -3620,7 +3848,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3632,18 +3860,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="D1" s="16" t="s">
+      <c r="B1" s="16"/>
+      <c r="D1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="G1" s="16" t="s">
+      <c r="E1" s="17"/>
+      <c r="G1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="16"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3673,16 +3901,16 @@
         <v>1450</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>113</v>
       </c>
       <c r="E3">
-        <v>1600</v>
+        <v>2000</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
       </c>
       <c r="H3">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -3701,21 +3929,24 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>2650</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
       </c>
       <c r="H5">
-        <v>600</v>
+        <v>550</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B6">
-        <v>6000</v>
+        <v>1100</v>
       </c>
       <c r="G6" t="s">
         <v>15</v>
@@ -3729,7 +3960,7 @@
         <v>24</v>
       </c>
       <c r="H7">
-        <v>1500</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3743,7 +3974,7 @@
       </c>
       <c r="E9">
         <f>SUM(E3:E8)</f>
-        <v>1600</v>
+        <v>2000</v>
       </c>
       <c r="G9" t="s">
         <v>73</v>
@@ -3755,25 +3986,25 @@
       </c>
       <c r="B10">
         <f>SUM(B3:B9)</f>
-        <v>8300</v>
+        <v>6050</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
       </c>
       <c r="H10">
         <f>SUM(H3:H9)</f>
-        <v>6500</v>
+        <v>4950</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="16"/>
+      <c r="B16" s="17"/>
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
     </row>
@@ -3800,21 +4031,13 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19">
-        <v>3400</v>
-      </c>
-    </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
       <c r="B23">
         <f>SUM(B18:B22)</f>
-        <v>18400</v>
+        <v>15000</v>
       </c>
     </row>
   </sheetData>
@@ -3853,18 +4076,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="D1" s="16" t="s">
+      <c r="B1" s="16"/>
+      <c r="D1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="G1" s="16" t="s">
+      <c r="E1" s="17"/>
+      <c r="G1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="16"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3894,10 +4117,10 @@
         <v>1450</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>113</v>
       </c>
       <c r="E3">
-        <v>950</v>
+        <v>1500</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -3908,10 +4131,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>4100</v>
+        <v>2650</v>
       </c>
       <c r="G4" t="s">
         <v>13</v>
@@ -3921,6 +4144,12 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5">
+        <v>900</v>
+      </c>
       <c r="G5" t="s">
         <v>14</v>
       </c>
@@ -3941,7 +4170,7 @@
         <v>24</v>
       </c>
       <c r="H7">
-        <v>1500</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3955,10 +4184,13 @@
       </c>
       <c r="E9">
         <f>SUM(E3:E8)</f>
-        <v>950</v>
+        <v>1500</v>
       </c>
       <c r="G9" t="s">
-        <v>73</v>
+        <v>96</v>
+      </c>
+      <c r="H9">
+        <v>500</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -3967,7 +4199,7 @@
       </c>
       <c r="B10">
         <f>SUM(B3:B9)</f>
-        <v>5550</v>
+        <v>5000</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
@@ -3978,14 +4210,14 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="16"/>
+      <c r="B16" s="17"/>
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
     </row>
@@ -4045,7 +4277,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4057,18 +4289,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="D1" s="16" t="s">
+      <c r="B1" s="16"/>
+      <c r="D1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="G1" s="16" t="s">
+      <c r="E1" s="17"/>
+      <c r="G1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="16"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -4097,19 +4329,25 @@
       <c r="B3">
         <v>1450</v>
       </c>
+      <c r="D3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3">
+        <v>1500</v>
+      </c>
       <c r="G3" t="s">
         <v>11</v>
       </c>
       <c r="H3">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>5550</v>
+        <v>2650</v>
       </c>
       <c r="G4" t="s">
         <v>13</v>
@@ -4119,6 +4357,12 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5">
+        <v>1900</v>
+      </c>
       <c r="G5" t="s">
         <v>14</v>
       </c>
@@ -4131,7 +4375,7 @@
         <v>15</v>
       </c>
       <c r="H6">
-        <v>1500</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -4139,7 +4383,7 @@
         <v>24</v>
       </c>
       <c r="H7">
-        <v>600</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -4153,13 +4397,13 @@
       </c>
       <c r="E9">
         <f>SUM(E3:E8)</f>
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="G9" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H9">
-        <v>1000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -4168,25 +4412,25 @@
       </c>
       <c r="B10">
         <f>SUM(B3:B9)</f>
-        <v>7000</v>
+        <v>6000</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
       </c>
       <c r="H10">
         <f>SUM(H3:H9)</f>
-        <v>6000</v>
+        <v>5500</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="16"/>
+      <c r="B16" s="17"/>
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
     </row>
@@ -4258,18 +4502,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="D1" s="16" t="s">
+      <c r="B1" s="16"/>
+      <c r="D1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="G1" s="16" t="s">
+      <c r="E1" s="17"/>
+      <c r="G1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="16"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -4296,7 +4540,13 @@
         <v>28</v>
       </c>
       <c r="B3">
-        <v>7000</v>
+        <v>1450</v>
+      </c>
+      <c r="D3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3">
+        <v>1500</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -4306,6 +4556,12 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>2650</v>
+      </c>
       <c r="G4" t="s">
         <v>13</v>
       </c>
@@ -4314,6 +4570,12 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5">
+        <v>900</v>
+      </c>
       <c r="G5" t="s">
         <v>14</v>
       </c>
@@ -4326,7 +4588,7 @@
         <v>15</v>
       </c>
       <c r="H6">
-        <v>1500</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -4334,7 +4596,7 @@
         <v>24</v>
       </c>
       <c r="H7">
-        <v>600</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -4348,13 +4610,13 @@
       </c>
       <c r="E9">
         <f>SUM(E3:E8)</f>
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="G9" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H9">
-        <v>1000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -4363,25 +4625,25 @@
       </c>
       <c r="B10">
         <f>SUM(B3:B9)</f>
-        <v>7000</v>
+        <v>5000</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
       </c>
       <c r="H10">
         <f>SUM(H3:H9)</f>
-        <v>6000</v>
+        <v>6500</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="16"/>
+      <c r="B16" s="17"/>
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
     </row>
@@ -4437,11 +4699,11 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8265F478-A579-4D4D-8C17-E927C389ADC0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDEB9995-7AFA-4020-994D-E08589C59BFF}">
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4453,18 +4715,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="D1" s="16" t="s">
+      <c r="B1" s="16"/>
+      <c r="D1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="G1" s="16" t="s">
+      <c r="E1" s="17"/>
+      <c r="G1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="16"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -4488,19 +4750,31 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="B3">
-        <v>7000</v>
+        <v>1450</v>
+      </c>
+      <c r="D3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3">
+        <v>1500</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
       </c>
       <c r="H3">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>2650</v>
+      </c>
       <c r="G4" t="s">
         <v>13</v>
       </c>
@@ -4509,6 +4783,12 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5">
+        <v>1900</v>
+      </c>
       <c r="G5" t="s">
         <v>14</v>
       </c>
@@ -4521,7 +4801,7 @@
         <v>15</v>
       </c>
       <c r="H6">
-        <v>1500</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -4529,7 +4809,7 @@
         <v>24</v>
       </c>
       <c r="H7">
-        <v>600</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -4543,13 +4823,13 @@
       </c>
       <c r="E9">
         <f>SUM(E3:E8)</f>
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="G9" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H9">
-        <v>1000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -4558,27 +4838,27 @@
       </c>
       <c r="B10">
         <f>SUM(B3:B9)</f>
-        <v>7000</v>
+        <v>6000</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
       </c>
       <c r="H10">
         <f>SUM(H3:H9)</f>
-        <v>6000</v>
+        <v>5500</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
+      <c r="B16" s="17"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -4587,7 +4867,7 @@
       <c r="B17" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="15" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4598,7 +4878,7 @@
       <c r="B18">
         <v>15000</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="15">
         <f>B23-B10-H10-E9</f>
         <v>2000</v>
       </c>
@@ -4646,14 +4926,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="E1" s="16" t="s">
+      <c r="B1" s="16"/>
+      <c r="E1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="16"/>
+      <c r="F1" s="17"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -4810,10 +5090,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="16"/>
+      <c r="B16" s="17"/>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -4873,11 +5153,644 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFECC3C-B62E-49F5-A68F-6241052BDF14}">
+  <dimension ref="A1:I23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="26.85546875" customWidth="1"/>
+    <col min="4" max="5" width="18.7109375" customWidth="1"/>
+    <col min="7" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="D1" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="17"/>
+      <c r="G1" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="17"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3">
+        <v>1450</v>
+      </c>
+      <c r="D3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3">
+        <v>1500</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>2650</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5">
+        <v>900</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <f>SUM(E3:E8)</f>
+        <v>1500</v>
+      </c>
+      <c r="G9" t="s">
+        <v>96</v>
+      </c>
+      <c r="H9">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <f>SUM(B3:B9)</f>
+        <v>5000</v>
+      </c>
+      <c r="G10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <f>SUM(H3:H9)</f>
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="17"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>15000</v>
+      </c>
+      <c r="E18" s="15">
+        <f>B23-B10-H10-E9</f>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <f>SUM(B18:B22)</f>
+        <v>15000</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="A16:B16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="5">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7896DF-CDEF-471C-A59C-7B910269B67F}">
+  <dimension ref="A1:I23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="26.85546875" customWidth="1"/>
+    <col min="4" max="5" width="18.7109375" customWidth="1"/>
+    <col min="7" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="D1" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="17"/>
+      <c r="G1" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="17"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3">
+        <v>1450</v>
+      </c>
+      <c r="D3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3">
+        <v>1500</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>2650</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5">
+        <v>1900</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <f>SUM(E3:E8)</f>
+        <v>1500</v>
+      </c>
+      <c r="G9" t="s">
+        <v>96</v>
+      </c>
+      <c r="H9">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <f>SUM(B3:B9)</f>
+        <v>6000</v>
+      </c>
+      <c r="G10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <f>SUM(H3:H9)</f>
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="17"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>15000</v>
+      </c>
+      <c r="E18" s="15">
+        <f>B23-B10-H10-E9</f>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <f>SUM(B18:B22)</f>
+        <v>15000</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="A16:B16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="5">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B65F810-9C84-4DE0-9AC5-AAEA1E957A65}">
+  <dimension ref="A1:I23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="26.85546875" customWidth="1"/>
+    <col min="4" max="5" width="18.7109375" customWidth="1"/>
+    <col min="7" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="D1" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="17"/>
+      <c r="G1" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="17"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>2650</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5">
+        <v>900</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6">
+        <v>2950</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <f>SUM(E3:E8)</f>
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>96</v>
+      </c>
+      <c r="H9">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <f>SUM(B3:B9)</f>
+        <v>6500</v>
+      </c>
+      <c r="G10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <f>SUM(H3:H9)</f>
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="17"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>15000</v>
+      </c>
+      <c r="E18" s="15">
+        <f>B23-B10-H10-E9</f>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <f>SUM(B18:B22)</f>
+        <v>15000</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="A16:B16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="5">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C91EC96-E704-492F-899B-E65E27E820DF}">
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A6" sqref="A6:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4887,10 +5800,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="15"/>
+      <c r="B1" s="16"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -5076,155 +5989,82 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FAE40A7-2F5B-4C6D-A8FB-C20244CB1571}">
-  <dimension ref="A1:E12"/>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E7693FE-503D-4498-AA09-7B77DD02E207}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="3" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>115</v>
       </c>
       <c r="B1" t="s">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>13000</v>
-      </c>
-      <c r="B2" s="6">
-        <v>1</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="6">
-        <v>2414</v>
-      </c>
-      <c r="E2" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2">
+        <v>3650</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3" s="6">
-        <v>2414</v>
-      </c>
-      <c r="E3" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="6">
+      <c r="B3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" s="6">
-        <v>2414</v>
-      </c>
-      <c r="E4" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="6">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>6700</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="6">
-        <v>2414</v>
-      </c>
-      <c r="E5" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="6">
-        <v>5</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" s="6">
-        <v>2414</v>
-      </c>
-      <c r="E6" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="6">
-        <v>6</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" s="6">
-        <v>2415</v>
-      </c>
-      <c r="E7" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="6">
-        <v>7</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D8" s="6">
-        <v>2415</v>
-      </c>
-      <c r="E8" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10">
-        <f>SUM(D2:D8)</f>
-        <v>16900</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12">
-        <f>D10-SUMIFS(D2:D8,E2:E8,"1")</f>
-        <v>0</v>
+      <c r="B5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <f>SUM(C2:C8)</f>
+        <v>15000</v>
       </c>
     </row>
   </sheetData>
@@ -5235,7 +6075,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52DEFC28-569B-4505-9F81-B6FB23EA0CD9}">
   <dimension ref="A1:E17"/>
   <sheetViews>
@@ -5458,7 +6298,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{814896F6-221A-4DF6-8B71-B3EAD3722806}">
   <dimension ref="A1:E17"/>
   <sheetViews>
@@ -5656,6 +6496,250 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FAE40A7-2F5B-4C6D-A8FB-C20244CB1571}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>13000</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="6">
+        <v>2414</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="6">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="6">
+        <v>2414</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="6">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="6">
+        <v>2414</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="6">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="6">
+        <v>2414</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="6">
+        <v>2414</v>
+      </c>
+      <c r="E6" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="6">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="6">
+        <v>2415</v>
+      </c>
+      <c r="E7" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="6">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="6">
+        <v>2415</v>
+      </c>
+      <c r="E8" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <f>SUM(D2:D8)</f>
+        <v>16900</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <f>D10-SUMIFS(D2:D8,E2:E8,"1")</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB7B190C-776A-4E01-8610-73C57EAD3F61}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="21.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>43723</v>
+      </c>
+      <c r="C2">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>43753</v>
+      </c>
+      <c r="C3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>43784</v>
+      </c>
+      <c r="C4">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>43814</v>
+      </c>
+      <c r="C5">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <f>SUM(C2:C8)</f>
+        <v>15000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80D55671-E077-47F0-8757-361362ABA21E}">
   <dimension ref="A1:H26"/>
@@ -5675,18 +6759,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="D1" s="16" t="s">
+      <c r="B1" s="16"/>
+      <c r="D1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="G1" s="16" t="s">
+      <c r="E1" s="17"/>
+      <c r="G1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="16"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -5812,16 +6896,16 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G16" s="16" t="s">
+      <c r="G16" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="H16" s="16"/>
+      <c r="H16" s="17"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="16"/>
+      <c r="B17" s="17"/>
       <c r="E17" s="2" t="s">
         <v>12</v>
       </c>
@@ -5938,18 +7022,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="D1" s="16" t="s">
+      <c r="B1" s="16"/>
+      <c r="D1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="G1" s="16" t="s">
+      <c r="E1" s="17"/>
+      <c r="G1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="16"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -6084,14 +7168,14 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="G16" s="16" t="s">
+      <c r="B16" s="17"/>
+      <c r="G16" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="H16" s="16"/>
+      <c r="H16" s="17"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -6198,18 +7282,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="D1" s="16" t="s">
+      <c r="B1" s="16"/>
+      <c r="D1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="G1" s="16" t="s">
+      <c r="E1" s="17"/>
+      <c r="G1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="16"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -6333,10 +7417,10 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="16"/>
+      <c r="B16" s="17"/>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -6421,18 +7505,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="D1" s="16" t="s">
+      <c r="B1" s="16"/>
+      <c r="D1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="G1" s="16" t="s">
+      <c r="E1" s="17"/>
+      <c r="G1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="16"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -6570,10 +7654,10 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="16"/>
+      <c r="B16" s="17"/>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -6642,18 +7726,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="D1" s="16" t="s">
+      <c r="B1" s="16"/>
+      <c r="D1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="G1" s="16" t="s">
+      <c r="E1" s="17"/>
+      <c r="G1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="16"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -6797,10 +7881,10 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="16"/>
+      <c r="B16" s="17"/>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -6877,18 +7961,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="D1" s="16" t="s">
+      <c r="B1" s="16"/>
+      <c r="D1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="G1" s="16" t="s">
+      <c r="E1" s="17"/>
+      <c r="G1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="16"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -7008,10 +8092,10 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="16"/>
+      <c r="B16" s="17"/>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -7082,18 +8166,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="D1" s="16" t="s">
+      <c r="B1" s="16"/>
+      <c r="D1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="G1" s="16" t="s">
+      <c r="E1" s="17"/>
+      <c r="G1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="16"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -7232,10 +8316,10 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G14" s="16" t="s">
+      <c r="G14" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="H14" s="16"/>
+      <c r="H14" s="17"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G15" t="s">
@@ -7249,10 +8333,10 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="16"/>
+      <c r="B16" s="17"/>
       <c r="G16" s="6" t="s">
         <v>6</v>
       </c>
@@ -7327,10 +8411,10 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="E21" s="16"/>
+      <c r="E21" s="17"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D22" t="s">

</xml_diff>

<commit_message>
Modificacion prestamo de kueski (5500) para pago inicial de la casa
</commit_message>
<xml_diff>
--- a/Counts_V3.xlsx
+++ b/Counts_V3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josuez-c\Desktop\Personal\Udemy\Git\Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C185F79-1A5C-4D76-BB84-2D004B1AB0C5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF58C09-2D1E-4419-81B0-9C4EDE09E40F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="13" activeTab="13" xr2:uid="{608168D3-9D0A-4B9A-96DD-5CA579F2C99B}"/>
+    <workbookView xWindow="2550" yWindow="1455" windowWidth="18045" windowHeight="12090" firstSheet="13" activeTab="15" xr2:uid="{608168D3-9D0A-4B9A-96DD-5CA579F2C99B}"/>
   </bookViews>
   <sheets>
     <sheet name="15 Feb" sheetId="3" r:id="rId1"/>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="125">
   <si>
     <t>Concepto</t>
   </si>
@@ -502,9 +502,6 @@
     <t>Prestamo 15K</t>
   </si>
   <si>
-    <t>Otras Deudas</t>
-  </si>
-  <si>
     <t>Otras-Deudas</t>
   </si>
   <si>
@@ -515,6 +512,21 @@
   </si>
   <si>
     <t>Neon</t>
+  </si>
+  <si>
+    <t>30 Septiembre</t>
+  </si>
+  <si>
+    <t>30 Octubre</t>
+  </si>
+  <si>
+    <t>30 Noviembre</t>
+  </si>
+  <si>
+    <t>30 Diciembre</t>
+  </si>
+  <si>
+    <t>Azgand</t>
   </si>
 </sst>
 </file>
@@ -1150,6 +1162,20 @@
 </file>
 
 <file path=xl/tables/table120.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="121" xr:uid="{04177E0B-0B25-4C62-A3A0-BA7129479543}" name="Table76122" displayName="Table76122" ref="A16:E26" totalsRowShown="0">
+  <autoFilter ref="A16:E26" xr:uid="{86DE9242-4569-4D2B-AE67-210BAD421B07}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{7953D040-6C9F-472F-9013-11158071C0FE}" name="Prestamo"/>
+    <tableColumn id="2" xr3:uid="{496AD683-3162-4ED8-970E-D68E6667AAA6}" name="Numero de abono"/>
+    <tableColumn id="3" xr3:uid="{A5948D2C-37BE-445C-A228-F80805DC060D}" name="Fecha"/>
+    <tableColumn id="4" xr3:uid="{4DA5AD81-C28F-4EAB-8AAF-C2D1972E8C03}" name="Pago Quincenal"/>
+    <tableColumn id="5" xr3:uid="{5E0297A8-C0F5-46B5-880C-91B85136CCA3}" name="Pagado"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table121.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="110" xr:uid="{B28A211B-7C8D-4126-9D65-5F77542B39C1}" name="Table172111" displayName="Table172111" ref="A1:C9" totalsRowShown="0">
   <autoFilter ref="A1:C9" xr:uid="{EF8E7F14-6CB0-4C4A-8A71-BFA9216C82C2}"/>
   <tableColumns count="3">
@@ -3422,7 +3448,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3632,8 +3658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D62384EF-D9B2-497E-AA08-6F8BC70A67AB}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3682,13 +3708,13 @@
       <c r="A3" t="s">
         <v>28</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="6">
         <v>1450</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="6">
         <v>7150</v>
       </c>
     </row>
@@ -3696,13 +3722,13 @@
       <c r="A4" t="s">
         <v>44</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="6">
         <v>850</v>
       </c>
       <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="6">
         <v>450</v>
       </c>
     </row>
@@ -3715,7 +3741,7 @@
       <c r="G6" t="s">
         <v>15</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="6">
         <v>2100</v>
       </c>
     </row>
@@ -3723,7 +3749,7 @@
       <c r="G7" t="s">
         <v>24</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="6">
         <v>1000</v>
       </c>
     </row>
@@ -3848,7 +3874,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3897,19 +3923,19 @@
       <c r="A3" t="s">
         <v>28</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="6">
         <v>1450</v>
       </c>
       <c r="D3" t="s">
         <v>113</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="6">
         <v>2000</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="6">
         <v>1000</v>
       </c>
     </row>
@@ -3931,7 +3957,7 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="6">
         <v>2650</v>
       </c>
       <c r="G5" t="s">
@@ -3951,7 +3977,7 @@
       <c r="G6" t="s">
         <v>15</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="6">
         <v>2100</v>
       </c>
     </row>
@@ -3959,7 +3985,7 @@
       <c r="G7" t="s">
         <v>24</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="6">
         <v>1000</v>
       </c>
     </row>
@@ -4063,8 +4089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3ADEAF8-8A81-4687-B9BC-AA53C493079B}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4113,63 +4139,63 @@
       <c r="A3" t="s">
         <v>28</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="6">
         <v>1450</v>
       </c>
       <c r="D3" t="s">
         <v>113</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="6">
         <v>1500</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="H3">
-        <v>2000</v>
+      <c r="H3" s="6">
+        <v>5900</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="6">
         <v>2650</v>
       </c>
       <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="H4">
-        <v>300</v>
-      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>29</v>
       </c>
       <c r="B5">
-        <v>900</v>
+        <v>1000</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
       </c>
-      <c r="H5">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" s="6">
         <v>600</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G6" t="s">
         <v>15</v>
       </c>
-      <c r="H6">
-        <v>2100</v>
+      <c r="H6" s="6">
+        <v>1800</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G7" t="s">
         <v>24</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="6">
         <v>1000</v>
       </c>
     </row>
@@ -4189,9 +4215,6 @@
       <c r="G9" t="s">
         <v>96</v>
       </c>
-      <c r="H9">
-        <v>500</v>
-      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -4199,14 +4222,14 @@
       </c>
       <c r="B10">
         <f>SUM(B3:B9)</f>
-        <v>5000</v>
+        <v>5700</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
       </c>
       <c r="H10">
         <f>SUM(H3:H9)</f>
-        <v>6500</v>
+        <v>8700</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -4244,13 +4267,21 @@
         <v>2000</v>
       </c>
     </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19">
+        <v>2900</v>
+      </c>
+    </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
       <c r="B23">
         <f>SUM(B18:B22)</f>
-        <v>15000</v>
+        <v>17900</v>
       </c>
     </row>
   </sheetData>
@@ -4277,7 +4308,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4339,7 +4370,7 @@
         <v>11</v>
       </c>
       <c r="H3">
-        <v>1000</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -4352,22 +4383,16 @@
       <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="H4">
-        <v>300</v>
-      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B5">
-        <v>1900</v>
+        <v>900</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
-      </c>
-      <c r="H5">
-        <v>600</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -4375,7 +4400,7 @@
         <v>15</v>
       </c>
       <c r="H6">
-        <v>2100</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -4402,9 +4427,6 @@
       <c r="G9" t="s">
         <v>96</v>
       </c>
-      <c r="H9">
-        <v>500</v>
-      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -4412,14 +4434,14 @@
       </c>
       <c r="B10">
         <f>SUM(B3:B9)</f>
-        <v>6000</v>
+        <v>5000</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
       </c>
       <c r="H10">
         <f>SUM(H3:H9)</f>
-        <v>5500</v>
+        <v>6500</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -4552,7 +4574,7 @@
         <v>11</v>
       </c>
       <c r="H3">
-        <v>2000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -4565,22 +4587,16 @@
       <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="H4">
-        <v>300</v>
-      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5">
         <v>900</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
-      </c>
-      <c r="H5">
-        <v>600</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -4588,7 +4604,7 @@
         <v>15</v>
       </c>
       <c r="H6">
-        <v>2100</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -4765,7 +4781,7 @@
         <v>11</v>
       </c>
       <c r="H3">
-        <v>1000</v>
+        <v>2600</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -4779,21 +4795,18 @@
         <v>13</v>
       </c>
       <c r="H4">
-        <v>300</v>
+        <v>400</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5">
-        <v>1900</v>
+        <v>900</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
-      </c>
-      <c r="H5">
-        <v>600</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -4801,7 +4814,7 @@
         <v>15</v>
       </c>
       <c r="H6">
-        <v>2100</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -4838,14 +4851,14 @@
       </c>
       <c r="B10">
         <f>SUM(B3:B9)</f>
-        <v>6000</v>
+        <v>5000</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
       </c>
       <c r="H10">
         <f>SUM(H3:H9)</f>
-        <v>5500</v>
+        <v>6500</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -5238,7 +5251,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5">
         <v>900</v>
@@ -5370,7 +5383,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5451,7 +5464,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5">
         <v>1900</v>
@@ -5652,7 +5665,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5">
         <v>900</v>
@@ -5790,7 +5803,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B9"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5849,7 +5862,7 @@
       </c>
       <c r="C4">
         <f>Laptop!D17</f>
-        <v>1670</v>
+        <v>835</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>28</v>
@@ -5975,7 +5988,7 @@
       </c>
       <c r="C13">
         <f>SUM(C3:C12)</f>
-        <v>9975</v>
+        <v>9140</v>
       </c>
     </row>
   </sheetData>
@@ -5993,9 +6006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E7693FE-503D-4498-AA09-7B77DD02E207}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6052,7 +6063,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C5">
         <v>650</v>
@@ -6079,7 +6090,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52DEFC28-569B-4505-9F81-B6FB23EA0CD9}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6251,14 +6264,17 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12">
+      <c r="B12" s="6">
         <v>11</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="6">
         <v>835</v>
+      </c>
+      <c r="E12" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -6287,7 +6303,7 @@
       </c>
       <c r="D17">
         <f>D15-SUMIFS(D2:D13,E2:E13,"1")</f>
-        <v>1670</v>
+        <v>835</v>
       </c>
     </row>
   </sheetData>
@@ -6498,7 +6514,7 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FAE40A7-2F5B-4C6D-A8FB-C20244CB1571}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6647,10 +6663,137 @@
         <v>0</v>
       </c>
     </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15000</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>121</v>
+      </c>
+      <c r="D20">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>122</v>
+      </c>
+      <c r="D22">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>123</v>
+      </c>
+      <c r="D24">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26">
+        <f>SUM(D17:D24)</f>
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28">
+        <f>D26-SUMIFS(D17:D23,E17:E23,"1")</f>
+        <v>21000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -6670,7 +6813,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B1" t="s">
         <v>65</v>

</xml_diff>

<commit_message>
Modificacion, terminar de pagar kuesky y kekipo en dic (modificacoin necesaria por cambio de casa), No la cagues
</commit_message>
<xml_diff>
--- a/Counts_V3.xlsx
+++ b/Counts_V3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josuez-c\Desktop\Personal\Udemy\Git\Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF58C09-2D1E-4419-81B0-9C4EDE09E40F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27018DC7-8FEB-4604-9DDD-53234D8F5D20}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="1455" windowWidth="18045" windowHeight="12090" firstSheet="13" activeTab="15" xr2:uid="{608168D3-9D0A-4B9A-96DD-5CA579F2C99B}"/>
+    <workbookView xWindow="9375" yWindow="1905" windowWidth="18045" windowHeight="12090" firstSheet="13" activeTab="16" xr2:uid="{608168D3-9D0A-4B9A-96DD-5CA579F2C99B}"/>
   </bookViews>
   <sheets>
     <sheet name="15 Feb" sheetId="3" r:id="rId1"/>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="128">
   <si>
     <t>Concepto</t>
   </si>
@@ -502,9 +502,6 @@
     <t>Prestamo 15K</t>
   </si>
   <si>
-    <t>Otras-Deudas</t>
-  </si>
-  <si>
     <t>Otras-deudas</t>
   </si>
   <si>
@@ -527,6 +524,18 @@
   </si>
   <si>
     <t>Azgand</t>
+  </si>
+  <si>
+    <t>TV</t>
+  </si>
+  <si>
+    <t>Edgar</t>
+  </si>
+  <si>
+    <t>Lesbiano</t>
+  </si>
+  <si>
+    <t>Otras Deudas</t>
   </si>
 </sst>
 </file>
@@ -3659,7 +3668,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6:H7"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3833,11 +3842,11 @@
         <v>2000</v>
       </c>
       <c r="H18">
-        <v>3400</v>
+        <v>6600</v>
       </c>
       <c r="I18">
         <f>(H18*I17)/H17</f>
-        <v>4681.9672131147545</v>
+        <v>9088.5245901639337</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -4089,8 +4098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3ADEAF8-8A81-4687-B9BC-AA53C493079B}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4145,14 +4154,11 @@
       <c r="D3" t="s">
         <v>113</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3">
         <v>1500</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
-      </c>
-      <c r="H3" s="6">
-        <v>5900</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -4162,13 +4168,19 @@
       <c r="B4" s="6">
         <v>2650</v>
       </c>
+      <c r="D4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1250</v>
+      </c>
       <c r="G4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B5">
         <v>1000</v>
@@ -4179,7 +4191,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B6" s="6">
         <v>600</v>
@@ -4188,10 +4200,16 @@
         <v>15</v>
       </c>
       <c r="H6" s="6">
-        <v>1800</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="6">
+        <v>5900</v>
+      </c>
       <c r="G7" t="s">
         <v>24</v>
       </c>
@@ -4210,7 +4228,7 @@
       </c>
       <c r="E9">
         <f>SUM(E3:E8)</f>
-        <v>1500</v>
+        <v>2750</v>
       </c>
       <c r="G9" t="s">
         <v>96</v>
@@ -4222,14 +4240,14 @@
       </c>
       <c r="B10">
         <f>SUM(B3:B9)</f>
-        <v>5700</v>
+        <v>11600</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
       </c>
       <c r="H10">
         <f>SUM(H3:H9)</f>
-        <v>8700</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -4264,7 +4282,7 @@
       </c>
       <c r="E18" s="13">
         <f>B23-B10-H10-E9</f>
-        <v>2000</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -4272,7 +4290,7 @@
         <v>7</v>
       </c>
       <c r="B19">
-        <v>2900</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -4281,7 +4299,7 @@
       </c>
       <c r="B23">
         <f>SUM(B18:B22)</f>
-        <v>17900</v>
+        <v>19000</v>
       </c>
     </row>
   </sheetData>
@@ -4307,8 +4325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AE4F4E1-7DCF-4B64-BE6C-12FCE9334F02}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4358,7 +4376,7 @@
         <v>28</v>
       </c>
       <c r="B3">
-        <v>1450</v>
+        <v>6000</v>
       </c>
       <c r="D3" t="s">
         <v>113</v>
@@ -4368,9 +4386,6 @@
       </c>
       <c r="G3" t="s">
         <v>11</v>
-      </c>
-      <c r="H3">
-        <v>3500</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -4386,16 +4401,22 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>900</v>
+        <v>4800</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6">
+        <v>800</v>
+      </c>
       <c r="G6" t="s">
         <v>15</v>
       </c>
@@ -4404,6 +4425,12 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7">
+        <v>324</v>
+      </c>
       <c r="G7" t="s">
         <v>24</v>
       </c>
@@ -4412,6 +4439,12 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8">
+        <v>500</v>
+      </c>
       <c r="G8" t="s">
         <v>53</v>
       </c>
@@ -4434,14 +4467,14 @@
       </c>
       <c r="B10">
         <f>SUM(B3:B9)</f>
-        <v>5000</v>
+        <v>15074</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
       </c>
       <c r="H10">
         <f>SUM(H3:H9)</f>
-        <v>6500</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -4476,7 +4509,15 @@
       </c>
       <c r="E18" s="13">
         <f>B23-B10-H10-E9</f>
-        <v>2000</v>
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19">
+        <v>6600</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -4485,7 +4526,7 @@
       </c>
       <c r="B23">
         <f>SUM(B18:B22)</f>
-        <v>15000</v>
+        <v>21600</v>
       </c>
     </row>
   </sheetData>
@@ -4561,9 +4602,6 @@
       <c r="A3" t="s">
         <v>28</v>
       </c>
-      <c r="B3">
-        <v>1450</v>
-      </c>
       <c r="D3" t="s">
         <v>113</v>
       </c>
@@ -4574,7 +4612,7 @@
         <v>11</v>
       </c>
       <c r="H3">
-        <v>3000</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -4590,10 +4628,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>900</v>
+        <v>7500</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
@@ -4631,9 +4669,6 @@
       <c r="G9" t="s">
         <v>96</v>
       </c>
-      <c r="H9">
-        <v>500</v>
-      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -4641,7 +4676,7 @@
       </c>
       <c r="B10">
         <f>SUM(B3:B9)</f>
-        <v>5000</v>
+        <v>10150</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
@@ -4683,7 +4718,15 @@
       </c>
       <c r="E18" s="13">
         <f>B23-B10-H10-E9</f>
-        <v>2000</v>
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19">
+        <v>5200</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -4692,7 +4735,7 @@
       </c>
       <c r="B23">
         <f>SUM(B18:B22)</f>
-        <v>15000</v>
+        <v>20200</v>
       </c>
     </row>
   </sheetData>
@@ -4765,12 +4808,6 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3">
-        <v>1450</v>
-      </c>
       <c r="D3" t="s">
         <v>113</v>
       </c>
@@ -4781,7 +4818,7 @@
         <v>11</v>
       </c>
       <c r="H3">
-        <v>2600</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -4800,10 +4837,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>900</v>
+        <v>6000</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
@@ -4841,9 +4878,6 @@
       <c r="G9" t="s">
         <v>96</v>
       </c>
-      <c r="H9">
-        <v>500</v>
-      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -4851,14 +4885,14 @@
       </c>
       <c r="B10">
         <f>SUM(B3:B9)</f>
-        <v>5000</v>
+        <v>8650</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
       </c>
       <c r="H10">
         <f>SUM(H3:H9)</f>
-        <v>6500</v>
+        <v>4900</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -4893,7 +4927,15 @@
       </c>
       <c r="E18" s="15">
         <f>B23-B10-H10-E9</f>
-        <v>2000</v>
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19">
+        <v>2100</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -4902,7 +4944,7 @@
       </c>
       <c r="B23">
         <f>SUM(B18:B22)</f>
-        <v>15000</v>
+        <v>17100</v>
       </c>
     </row>
   </sheetData>
@@ -5219,9 +5261,6 @@
       <c r="A3" t="s">
         <v>28</v>
       </c>
-      <c r="B3">
-        <v>1450</v>
-      </c>
       <c r="D3" t="s">
         <v>113</v>
       </c>
@@ -5251,19 +5290,22 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>900</v>
+        <v>3000</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
       </c>
-      <c r="H5">
-        <v>600</v>
-      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6">
+        <v>450</v>
+      </c>
       <c r="G6" t="s">
         <v>15</v>
       </c>
@@ -5295,9 +5337,6 @@
       <c r="G9" t="s">
         <v>96</v>
       </c>
-      <c r="H9">
-        <v>500</v>
-      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -5305,14 +5344,14 @@
       </c>
       <c r="B10">
         <f>SUM(B3:B9)</f>
-        <v>5000</v>
+        <v>6100</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
       </c>
       <c r="H10">
         <f>SUM(H3:H9)</f>
-        <v>6500</v>
+        <v>5400</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -5383,7 +5422,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5432,9 +5471,6 @@
       <c r="A3" t="s">
         <v>28</v>
       </c>
-      <c r="B3">
-        <v>1450</v>
-      </c>
       <c r="D3" t="s">
         <v>113</v>
       </c>
@@ -5445,7 +5481,7 @@
         <v>11</v>
       </c>
       <c r="H3">
-        <v>1000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -5464,16 +5500,13 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B5">
-        <v>1900</v>
+        <v>3950</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
-      </c>
-      <c r="H5">
-        <v>600</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -5508,9 +5541,6 @@
       <c r="G9" t="s">
         <v>96</v>
       </c>
-      <c r="H9">
-        <v>500</v>
-      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -5518,14 +5548,14 @@
       </c>
       <c r="B10">
         <f>SUM(B3:B9)</f>
-        <v>6000</v>
+        <v>6600</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
       </c>
       <c r="H10">
         <f>SUM(H3:H9)</f>
-        <v>5500</v>
+        <v>4900</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -5665,25 +5695,16 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B5">
-        <v>900</v>
+        <v>4950</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
       </c>
-      <c r="H5">
-        <v>600</v>
-      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6">
-        <v>2950</v>
-      </c>
       <c r="G6" t="s">
         <v>15</v>
       </c>
@@ -5715,9 +5736,6 @@
       <c r="G9" t="s">
         <v>96</v>
       </c>
-      <c r="H9">
-        <v>500</v>
-      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -5725,14 +5743,14 @@
       </c>
       <c r="B10">
         <f>SUM(B3:B9)</f>
-        <v>6500</v>
+        <v>7600</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
       </c>
       <c r="H10">
         <f>SUM(H3:H9)</f>
-        <v>6500</v>
+        <v>5400</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -6063,7 +6081,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C5">
         <v>650</v>
@@ -6699,7 +6717,7 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D18">
         <v>2625</v>
@@ -6721,7 +6739,7 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D20">
         <v>2625</v>
@@ -6743,7 +6761,7 @@
         <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D22">
         <v>2625</v>
@@ -6765,7 +6783,7 @@
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D24">
         <v>2625</v>
@@ -6813,7 +6831,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
         <v>65</v>

</xml_diff>

<commit_message>
Ajustando pagos de Kekipo, y estimaciones de proximos pagos
</commit_message>
<xml_diff>
--- a/Counts_V3.xlsx
+++ b/Counts_V3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josuez-c\Desktop\Personal\Udemy\Git\Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27018DC7-8FEB-4604-9DDD-53234D8F5D20}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24C7AE0-2C94-41F3-A694-B390916E3E51}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9375" yWindow="1905" windowWidth="18045" windowHeight="12090" firstSheet="13" activeTab="16" xr2:uid="{608168D3-9D0A-4B9A-96DD-5CA579F2C99B}"/>
+    <workbookView xWindow="5805" yWindow="300" windowWidth="18690" windowHeight="12720" firstSheet="16" activeTab="16" xr2:uid="{608168D3-9D0A-4B9A-96DD-5CA579F2C99B}"/>
   </bookViews>
   <sheets>
     <sheet name="15 Feb" sheetId="3" r:id="rId1"/>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="130">
   <si>
     <t>Concepto</t>
   </si>
@@ -536,6 +536,12 @@
   </si>
   <si>
     <t>Otras Deudas</t>
+  </si>
+  <si>
+    <t>Colunga</t>
+  </si>
+  <si>
+    <t>Kueski Estimacion (15 dias)</t>
   </si>
 </sst>
 </file>
@@ -639,7 +645,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -667,6 +673,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -676,7 +685,16 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="67">
+  <dxfs count="70">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -914,6 +932,30 @@
 </file>
 
 <file path=xl/tables/table100.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="89" xr:uid="{CB35E77C-BB8D-4BF0-A025-005D8F6CD22E}" name="Table434546474849515661667183899510010590" displayName="Table434546474849515661667183899510010590" ref="D2:E9" totalsRowShown="0">
+  <autoFilter ref="D2:E9" xr:uid="{35909676-23EE-45B1-96DF-AD227C9C3285}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{38930260-C22E-447F-BC3C-5F385FDA2E16}" name="Concepto"/>
+    <tableColumn id="2" xr3:uid="{88ACDE1C-DE29-4B11-8592-5C39F1030437}" name="Monto"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table101.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="123" xr:uid="{8CE4229E-B39F-4C1B-83DA-3078678A7407}" name="Table83123124" displayName="Table83123124" ref="G18:H20" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="G18:H20" xr:uid="{3C807007-B87E-4A98-B721-D14C621DC426}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{47087C85-33C9-470D-B1FC-57277678895D}" name="Monto Pedido"/>
+    <tableColumn id="2" xr3:uid="{82A952D9-5737-47F8-AB35-348F25CBA81D}" name="Monto a pagar (Aprox)">
+      <calculatedColumnFormula>(G19*H18)/G18</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table102.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="105" xr:uid="{BD444082-668C-465E-8E5A-2648EDC88476}" name="Table161014192327313539525762675859196101106" displayName="Table161014192327313539525762675859196101106" ref="A2:B10" totalsRowShown="0">
   <autoFilter ref="A2:B10" xr:uid="{118E6C9A-65CE-41B2-9CDA-E2E803A2ACA4}"/>
   <tableColumns count="2">
@@ -924,7 +966,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table101.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table103.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="106" xr:uid="{77629009-D81D-4AC6-AAFD-5A6E426D1416}" name="Table2711152024283236405358636880869297102107" displayName="Table2711152024283236405358636880869297102107" ref="G2:H10" totalsRowShown="0">
   <autoFilter ref="G2:H10" xr:uid="{55D0E6FB-2E76-4927-9D34-9CAA769EF7F7}"/>
   <tableColumns count="2">
@@ -935,7 +977,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table102.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table104.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="107" xr:uid="{BA84FDCA-BD7E-4196-892D-B3329C234F27}" name="Table712162125293337415459646981879398103108" displayName="Table712162125293337415459646981879398103108" ref="A17:B23" totalsRowShown="0">
   <autoFilter ref="A17:B23" xr:uid="{5ACFFE3C-8C54-4A57-BCD6-735E5CE8DEA7}"/>
   <tableColumns count="2">
@@ -946,11 +988,11 @@
 </table>
 </file>
 
-<file path=xl/tables/table103.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="108" xr:uid="{4031720E-0F95-4EA7-850B-4816832DE48D}" name="Table813172226303438425560657082889499104109" displayName="Table813172226303438425560657082889499104109" ref="E17:E18" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<file path=xl/tables/table105.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="108" xr:uid="{4031720E-0F95-4EA7-850B-4816832DE48D}" name="Table813172226303438425560657082889499104109" displayName="Table813172226303438425560657082889499104109" ref="E17:E18" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{AA136418-89BA-4512-8280-2F80F616CFFF}" name="Restante" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{AA136418-89BA-4512-8280-2F80F616CFFF}" name="Restante" dataDxfId="9">
       <calculatedColumnFormula>B23-B10-H10-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -958,7 +1000,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table104.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table106.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="109" xr:uid="{65772710-F64D-4FB6-BA14-124D521E900F}" name="Table4345464748495156616671838995100105110" displayName="Table4345464748495156616671838995100105110" ref="D2:E9" totalsRowShown="0">
   <autoFilter ref="D2:E9" xr:uid="{35909676-23EE-45B1-96DF-AD227C9C3285}"/>
   <tableColumns count="2">
@@ -969,7 +1011,20 @@
 </table>
 </file>
 
-<file path=xl/tables/table105.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table107.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="124" xr:uid="{ECB75F05-103B-49D8-8133-EA28FFF12D2F}" name="Table83123124125" displayName="Table83123124125" ref="G18:H20" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="G18:H20" xr:uid="{F8C1B37A-07DB-47EB-BB6F-128432BD8FDC}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{D5193CCF-D1B9-4151-A6EA-3BD48B330D1B}" name="Monto Pedido"/>
+    <tableColumn id="2" xr3:uid="{F0B92D08-C0D8-4A24-8B3A-C69E1C44E2E2}" name="Monto a pagar (Aprox)">
+      <calculatedColumnFormula>(G19*H18)/G18</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table108.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="111" xr:uid="{1CFA8894-1C3C-421D-8413-EBEA7B4934DC}" name="Table16101419232731353952576267585919610173112" displayName="Table16101419232731353952576267585919610173112" ref="A2:B10" totalsRowShown="0">
   <autoFilter ref="A2:B10" xr:uid="{118E6C9A-65CE-41B2-9CDA-E2E803A2ACA4}"/>
   <tableColumns count="2">
@@ -980,7 +1035,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table106.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table109.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="112" xr:uid="{7EBAB4EB-5E5A-41F2-B35A-2D97BEB3C845}" name="Table271115202428323640535863688086929710274113" displayName="Table271115202428323640535863688086929710274113" ref="G2:H10" totalsRowShown="0">
   <autoFilter ref="G2:H10" xr:uid="{55D0E6FB-2E76-4927-9D34-9CAA769EF7F7}"/>
   <tableColumns count="2">
@@ -988,40 +1043,6 @@
     <tableColumn id="2" xr3:uid="{52FA1AFE-C6CC-4A87-84CB-62802F9DD0CE}" name="Monto"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table107.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="113" xr:uid="{423080DD-CE5C-480C-BB58-136905C750E2}" name="Table71216212529333741545964698187939810375114" displayName="Table71216212529333741545964698187939810375114" ref="A17:B23" totalsRowShown="0">
-  <autoFilter ref="A17:B23" xr:uid="{5ACFFE3C-8C54-4A57-BCD6-735E5CE8DEA7}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{D40B5449-BE47-4077-BC63-8C4BA29EF00A}" name="Concepto"/>
-    <tableColumn id="2" xr3:uid="{408F9E12-BBAB-46FC-BC70-BFFC091A5DA1}" name="Monto"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table108.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="114" xr:uid="{E34FDC91-9B3B-449A-9349-4982300F405D}" name="Table81317222630343842556065708288949910476115" displayName="Table81317222630343842556065708288949910476115" ref="E17:E18" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{87008DBD-1138-46AC-AEB4-2C20ADBEBD05}" name="Restante" dataDxfId="3">
-      <calculatedColumnFormula>B23-B10-H10-E9</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table109.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="115" xr:uid="{77B1E7DE-A265-482D-8830-C92FA0E9E23F}" name="Table434546474849515661667183899510010590116" displayName="Table434546474849515661667183899510010590116" ref="D2:E9" totalsRowShown="0">
-  <autoFilter ref="D2:E9" xr:uid="{35909676-23EE-45B1-96DF-AD227C9C3285}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{CDD8F792-B0C8-41ED-9960-F6F2A0326FCF}" name="Concepto"/>
-    <tableColumn id="2" xr3:uid="{F9D65851-DEE4-4F7D-B525-0830553B6180}" name="Monto"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1037,6 +1058,40 @@
 </file>
 
 <file path=xl/tables/table110.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="113" xr:uid="{423080DD-CE5C-480C-BB58-136905C750E2}" name="Table71216212529333741545964698187939810375114" displayName="Table71216212529333741545964698187939810375114" ref="A17:B23" totalsRowShown="0">
+  <autoFilter ref="A17:B23" xr:uid="{5ACFFE3C-8C54-4A57-BCD6-735E5CE8DEA7}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{D40B5449-BE47-4077-BC63-8C4BA29EF00A}" name="Concepto"/>
+    <tableColumn id="2" xr3:uid="{408F9E12-BBAB-46FC-BC70-BFFC091A5DA1}" name="Monto"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table111.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="114" xr:uid="{E34FDC91-9B3B-449A-9349-4982300F405D}" name="Table81317222630343842556065708288949910476115" displayName="Table81317222630343842556065708288949910476115" ref="E17:E18" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{87008DBD-1138-46AC-AEB4-2C20ADBEBD05}" name="Restante" dataDxfId="6">
+      <calculatedColumnFormula>B23-B10-H10-E9</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table112.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="115" xr:uid="{77B1E7DE-A265-482D-8830-C92FA0E9E23F}" name="Table434546474849515661667183899510010590116" displayName="Table434546474849515661667183899510010590116" ref="D2:E9" totalsRowShown="0">
+  <autoFilter ref="D2:E9" xr:uid="{35909676-23EE-45B1-96DF-AD227C9C3285}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{CDD8F792-B0C8-41ED-9960-F6F2A0326FCF}" name="Concepto"/>
+    <tableColumn id="2" xr3:uid="{F9D65851-DEE4-4F7D-B525-0830553B6180}" name="Monto"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table113.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="116" xr:uid="{1D95C88F-0BBF-49F3-85FE-40AC1BE32AB4}" name="Table161014192327313539525762675859196101106117" displayName="Table161014192327313539525762675859196101106117" ref="A2:B10" totalsRowShown="0">
   <autoFilter ref="A2:B10" xr:uid="{118E6C9A-65CE-41B2-9CDA-E2E803A2ACA4}"/>
   <tableColumns count="2">
@@ -1047,7 +1102,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table111.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table114.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="117" xr:uid="{2BD61BFA-F743-4712-A73F-CAAE8DA445E9}" name="Table2711152024283236405358636880869297102107118" displayName="Table2711152024283236405358636880869297102107118" ref="G2:H10" totalsRowShown="0">
   <autoFilter ref="G2:H10" xr:uid="{55D0E6FB-2E76-4927-9D34-9CAA769EF7F7}"/>
   <tableColumns count="2">
@@ -1058,7 +1113,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table112.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table115.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="118" xr:uid="{D4A4AE6F-D5A5-41CB-B1B7-E520F7E7A0EA}" name="Table712162125293337415459646981879398103108119" displayName="Table712162125293337415459646981879398103108119" ref="A17:B23" totalsRowShown="0">
   <autoFilter ref="A17:B23" xr:uid="{5ACFFE3C-8C54-4A57-BCD6-735E5CE8DEA7}"/>
   <tableColumns count="2">
@@ -1069,11 +1124,11 @@
 </table>
 </file>
 
-<file path=xl/tables/table113.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="119" xr:uid="{47E7B440-9775-4359-A21B-8717CD3589CE}" name="Table813172226303438425560657082889499104109120" displayName="Table813172226303438425560657082889499104109120" ref="E17:E18" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+<file path=xl/tables/table116.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="119" xr:uid="{47E7B440-9775-4359-A21B-8717CD3589CE}" name="Table813172226303438425560657082889499104109120" displayName="Table813172226303438425560657082889499104109120" ref="E17:E18" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{6B7F805A-0C9D-4169-8EB3-B8D113010DB4}" name="Restante" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{6B7F805A-0C9D-4169-8EB3-B8D113010DB4}" name="Restante" dataDxfId="3">
       <calculatedColumnFormula>B23-B10-H10-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1081,7 +1136,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table114.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table117.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="120" xr:uid="{E407E054-CDD6-421B-B619-8CE8355F8C8D}" name="Table4345464748495156616671838995100105110121" displayName="Table4345464748495156616671838995100105110121" ref="D2:E9" totalsRowShown="0">
   <autoFilter ref="D2:E9" xr:uid="{35909676-23EE-45B1-96DF-AD227C9C3285}"/>
   <tableColumns count="2">
@@ -1092,7 +1147,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table115.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table118.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{A7428449-465F-4335-8A22-A04831709D07}" name="Table1618" displayName="Table1618" ref="A2:C13" totalsRowShown="0">
   <autoFilter ref="A2:C13" xr:uid="{A4206556-B7C7-4E7D-80ED-F4D40D255729}"/>
   <tableColumns count="3">
@@ -1104,7 +1159,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table116.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table119.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="71" xr:uid="{C1E6F83D-8473-4577-9A45-6FA8E84217EA}" name="Table172" displayName="Table172" ref="A1:C9" totalsRowShown="0">
   <autoFilter ref="A1:C9" xr:uid="{E85945BF-0347-4283-B4FB-329C892B49AD}"/>
   <tableColumns count="3">
@@ -1116,7 +1171,19 @@
 </table>
 </file>
 
-<file path=xl/tables/table117.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{6EB74B2F-5FCA-473F-9FAA-3EDF8111D5D5}" name="Table81317" displayName="Table81317" ref="E17:E18" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
+  <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{CE9482A1-3934-4F51-997A-9EFBA1863710}" name="Restante" dataDxfId="61">
+      <calculatedColumnFormula>B24-B9-H9-E9</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table120.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="77" xr:uid="{45800315-40D0-4619-A718-EF9AD896042B}" name="Table7678" displayName="Table7678" ref="A1:E15" totalsRowShown="0">
   <autoFilter ref="A1:E15" xr:uid="{3D62BFF4-E1EC-48EF-8175-8365BDEB915E}"/>
   <tableColumns count="5">
@@ -1130,7 +1197,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table118.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table121.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="78" xr:uid="{C37A6D5E-2C67-42BD-A506-B21D8F530A79}" name="Table767879" displayName="Table767879" ref="A1:E15" totalsRowShown="0">
   <autoFilter ref="A1:E15" xr:uid="{3D62BFF4-E1EC-48EF-8175-8365BDEB915E}"/>
   <tableColumns count="5">
@@ -1144,7 +1211,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table119.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table122.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="76" xr:uid="{97221669-6CC7-4845-8A50-42C4FBDBF442}" name="Table76" displayName="Table76" ref="A1:E10" totalsRowShown="0">
   <autoFilter ref="A1:E10" xr:uid="{3D62BFF4-E1EC-48EF-8175-8365BDEB915E}"/>
   <tableColumns count="5">
@@ -1158,19 +1225,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{6EB74B2F-5FCA-473F-9FAA-3EDF8111D5D5}" name="Table81317" displayName="Table81317" ref="E17:E18" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
-  <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{CE9482A1-3934-4F51-997A-9EFBA1863710}" name="Restante" dataDxfId="58">
-      <calculatedColumnFormula>B24-B9-H9-E9</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table120.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table123.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="121" xr:uid="{04177E0B-0B25-4C62-A3A0-BA7129479543}" name="Table76122" displayName="Table76122" ref="A16:E26" totalsRowShown="0">
   <autoFilter ref="A16:E26" xr:uid="{86DE9242-4569-4D2B-AE67-210BAD421B07}"/>
   <tableColumns count="5">
@@ -1184,7 +1239,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table121.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table124.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="110" xr:uid="{B28A211B-7C8D-4126-9D65-5F77542B39C1}" name="Table172111" displayName="Table172111" ref="A1:C9" totalsRowShown="0">
   <autoFilter ref="A1:C9" xr:uid="{EF8E7F14-6CB0-4C4A-8A71-BFA9216C82C2}"/>
   <tableColumns count="3">
@@ -1252,10 +1307,10 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{C6113CAB-14DB-4CA9-B83E-7B558420A38C}" name="Table8131722" displayName="Table8131722" ref="E17:E18" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{C6113CAB-14DB-4CA9-B83E-7B558420A38C}" name="Table8131722" displayName="Table8131722" ref="E17:E18" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{17B47C4D-B270-4929-9F44-5483826CC1AE}" name="Restante" dataDxfId="55">
+    <tableColumn id="1" xr3:uid="{17B47C4D-B270-4929-9F44-5483826CC1AE}" name="Restante" dataDxfId="58">
       <calculatedColumnFormula>B23-B11-H9-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1330,10 +1385,10 @@
 </file>
 
 <file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{F627F082-294B-4972-9027-409731C849B1}" name="Table813172226" displayName="Table813172226" ref="E17:E18" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{F627F082-294B-4972-9027-409731C849B1}" name="Table813172226" displayName="Table813172226" ref="E17:E18" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{84805B74-C396-407D-B3EF-AA50F3B88793}" name="Restante" dataDxfId="52">
+    <tableColumn id="1" xr3:uid="{84805B74-C396-407D-B3EF-AA50F3B88793}" name="Restante" dataDxfId="55">
       <calculatedColumnFormula>B23-B11-H9-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1386,10 +1441,10 @@
 </file>
 
 <file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{F2237E1E-DB59-4357-9ED1-E146B786B6E8}" name="Table81317222630" displayName="Table81317222630" ref="E17:E18" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{F2237E1E-DB59-4357-9ED1-E146B786B6E8}" name="Table81317222630" displayName="Table81317222630" ref="E17:E18" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{7FE38D7A-746A-4B78-86EA-E6C48DDBB8A0}" name="Restante" dataDxfId="49">
+    <tableColumn id="1" xr3:uid="{7FE38D7A-746A-4B78-86EA-E6C48DDBB8A0}" name="Restante" dataDxfId="52">
       <calculatedColumnFormula>B23-B11-H9-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1453,10 +1508,10 @@
 </file>
 
 <file path=xl/tables/table34.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{B70A0F6A-8050-4DB3-85A2-CB613921E543}" name="Table8131722263034" displayName="Table8131722263034" ref="E17:E18" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{B70A0F6A-8050-4DB3-85A2-CB613921E543}" name="Table8131722263034" displayName="Table8131722263034" ref="E17:E18" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{291FFC4C-53BF-4611-8650-189C4CE99ED2}" name="Restante" dataDxfId="46">
+    <tableColumn id="1" xr3:uid="{291FFC4C-53BF-4611-8650-189C4CE99ED2}" name="Restante" dataDxfId="49">
       <calculatedColumnFormula>B23-B11-H9-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1509,10 +1564,10 @@
 </file>
 
 <file path=xl/tables/table39.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="37" xr:uid="{6CE768FB-536E-4602-8FA1-80E57812D3D7}" name="Table813172226303438" displayName="Table813172226303438" ref="E17:E18" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="37" xr:uid="{6CE768FB-536E-4602-8FA1-80E57812D3D7}" name="Table813172226303438" displayName="Table813172226303438" ref="E17:E18" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{6A83FD00-1A49-4187-B78E-59E702BF0D8C}" name="Restante" dataDxfId="43">
+    <tableColumn id="1" xr3:uid="{6A83FD00-1A49-4187-B78E-59E702BF0D8C}" name="Restante" dataDxfId="46">
       <calculatedColumnFormula>B23-B11-H9-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1521,10 +1576,10 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{CF7189AF-8506-457B-AF02-678238446516}" name="Table8" displayName="Table8" ref="F14:F15" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{CF7189AF-8506-457B-AF02-678238446516}" name="Table8" displayName="Table8" ref="F14:F15" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68">
   <autoFilter ref="F14:F15" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{4A560B8E-4A45-4A34-80BB-77B5C3912F5F}" name="Restante" dataDxfId="64">
+    <tableColumn id="1" xr3:uid="{4A560B8E-4A45-4A34-80BB-77B5C3912F5F}" name="Restante" dataDxfId="67">
       <calculatedColumnFormula>B21-B10-F10</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1577,10 +1632,10 @@
 </file>
 
 <file path=xl/tables/table44.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="41" xr:uid="{221D2EBC-F3BE-4FFD-BA8C-2A7B2D5F1F06}" name="Table81317222630343842" displayName="Table81317222630343842" ref="E17:E18" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="41" xr:uid="{221D2EBC-F3BE-4FFD-BA8C-2A7B2D5F1F06}" name="Table81317222630343842" displayName="Table81317222630343842" ref="E17:E18" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{C983AC74-910C-462A-A5AC-E4E7D8251DD7}" name="Restante" dataDxfId="40">
+    <tableColumn id="1" xr3:uid="{C983AC74-910C-462A-A5AC-E4E7D8251DD7}" name="Restante" dataDxfId="43">
       <calculatedColumnFormula>B23-B10-H9-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1677,10 +1732,10 @@
 </file>
 
 <file path=xl/tables/table52.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="54" xr:uid="{D8CF4A15-7D2D-43A1-BDCD-6886F425BACE}" name="Table8131722263034384255" displayName="Table8131722263034384255" ref="E17:E18" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="54" xr:uid="{D8CF4A15-7D2D-43A1-BDCD-6886F425BACE}" name="Table8131722263034384255" displayName="Table8131722263034384255" ref="E17:E18" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{01FC21D7-E33E-4541-80CD-10112E5DAD8E}" name="Restante" dataDxfId="37">
+    <tableColumn id="1" xr3:uid="{01FC21D7-E33E-4541-80CD-10112E5DAD8E}" name="Restante" dataDxfId="40">
       <calculatedColumnFormula>B23-B10-H9-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1733,10 +1788,10 @@
 </file>
 
 <file path=xl/tables/table57.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="59" xr:uid="{78652AD3-F12D-41C4-B189-0D7B21314932}" name="Table813172226303438425560" displayName="Table813172226303438425560" ref="E17:E18" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="59" xr:uid="{78652AD3-F12D-41C4-B189-0D7B21314932}" name="Table813172226303438425560" displayName="Table813172226303438425560" ref="E17:E18" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{3E662EAE-9351-4FAF-8E50-D47E45AE97AC}" name="Restante" dataDxfId="34">
+    <tableColumn id="1" xr3:uid="{3E662EAE-9351-4FAF-8E50-D47E45AE97AC}" name="Restante" dataDxfId="37">
       <calculatedColumnFormula>B23-B10-H9-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1800,10 +1855,10 @@
 </file>
 
 <file path=xl/tables/table62.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="64" xr:uid="{B957AF75-42E6-4BA6-9FC2-1F38625FFD28}" name="Table81317222630343842556065" displayName="Table81317222630343842556065" ref="E17:E18" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="64" xr:uid="{B957AF75-42E6-4BA6-9FC2-1F38625FFD28}" name="Table81317222630343842556065" displayName="Table81317222630343842556065" ref="E17:E18" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{FB468390-A346-49F3-B226-62B380F4E00B}" name="Restante" dataDxfId="31">
+    <tableColumn id="1" xr3:uid="{FB468390-A346-49F3-B226-62B380F4E00B}" name="Restante" dataDxfId="34">
       <calculatedColumnFormula>B23-B10-H10-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1856,10 +1911,10 @@
 </file>
 
 <file path=xl/tables/table67.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="69" xr:uid="{1F763CB0-5D67-4782-B1D1-185995FAF701}" name="Table8131722263034384255606570" displayName="Table8131722263034384255606570" ref="E17:E18" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="69" xr:uid="{1F763CB0-5D67-4782-B1D1-185995FAF701}" name="Table8131722263034384255606570" displayName="Table8131722263034384255606570" ref="E17:E18" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{015756F4-B40A-45B4-A6BD-967346B724AB}" name="Restante" dataDxfId="28">
+    <tableColumn id="1" xr3:uid="{015756F4-B40A-45B4-A6BD-967346B724AB}" name="Restante" dataDxfId="31">
       <calculatedColumnFormula>B23-B10-H10-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1923,10 +1978,10 @@
 </file>
 
 <file path=xl/tables/table72.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="81" xr:uid="{03938C9E-C130-4923-AEFB-4E7EE2A4779E}" name="Table813172226303438425560657082" displayName="Table813172226303438425560657082" ref="E17:E18" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="81" xr:uid="{03938C9E-C130-4923-AEFB-4E7EE2A4779E}" name="Table813172226303438425560657082" displayName="Table813172226303438425560657082" ref="E17:E18" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{36023DA8-4FE9-47DD-B333-A9AFE4EB7204}" name="Restante" dataDxfId="25">
+    <tableColumn id="1" xr3:uid="{36023DA8-4FE9-47DD-B333-A9AFE4EB7204}" name="Restante" dataDxfId="28">
       <calculatedColumnFormula>B23-B10-H10-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1946,7 +2001,7 @@
 </file>
 
 <file path=xl/tables/table74.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="83" xr:uid="{2AF05975-5D9A-45C8-920B-D15CCD6D82B8}" name="Table83" displayName="Table83" ref="H16:I18" totalsRowShown="0" headerRowDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="83" xr:uid="{2AF05975-5D9A-45C8-920B-D15CCD6D82B8}" name="Table83" displayName="Table83" ref="H16:I18" totalsRowShown="0" headerRowDxfId="27">
   <autoFilter ref="H16:I18" xr:uid="{858BF2D4-21A7-4045-A21A-FA9333CB1404}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{98539052-BA4D-4533-AF09-70C6F2D918B6}" name="Monto Pedido"/>
@@ -1992,10 +2047,10 @@
 </file>
 
 <file path=xl/tables/table78.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="87" xr:uid="{E7FB8AF9-F2FC-41D6-A5E7-C62FD5A65876}" name="Table81317222630343842556065708288" displayName="Table81317222630343842556065708288" ref="E17:E18" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="87" xr:uid="{E7FB8AF9-F2FC-41D6-A5E7-C62FD5A65876}" name="Table81317222630343842556065708288" displayName="Table81317222630343842556065708288" ref="E17:E18" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{22311529-0E6B-4E18-B7B7-AABA36467ADA}" name="Restante" dataDxfId="21">
+    <tableColumn id="1" xr3:uid="{22311529-0E6B-4E18-B7B7-AABA36467ADA}" name="Restante" dataDxfId="24">
       <calculatedColumnFormula>B23-B10-H10-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2015,10 +2070,10 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{94410419-2417-4F8D-990A-61DB66FE296E}" name="Table813" displayName="Table813" ref="F17:F18" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{94410419-2417-4F8D-990A-61DB66FE296E}" name="Table813" displayName="Table813" ref="F17:F18" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
   <autoFilter ref="F17:F18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{02ABE55D-D08A-4FAB-9216-A7A6F25790A3}" name="Restante" dataDxfId="61">
+    <tableColumn id="1" xr3:uid="{02ABE55D-D08A-4FAB-9216-A7A6F25790A3}" name="Restante" dataDxfId="64">
       <calculatedColumnFormula>B23-C12-F9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2060,10 +2115,10 @@
 </file>
 
 <file path=xl/tables/table83.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="93" xr:uid="{6FA57C93-C1AB-4452-8152-77D321556756}" name="Table8131722263034384255606570828894" displayName="Table8131722263034384255606570828894" ref="E17:E18" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="93" xr:uid="{6FA57C93-C1AB-4452-8152-77D321556756}" name="Table8131722263034384255606570828894" displayName="Table8131722263034384255606570828894" ref="E17:E18" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{823C011F-989F-468A-98EA-B63D69D1F99D}" name="Restante" dataDxfId="18">
+    <tableColumn id="1" xr3:uid="{823C011F-989F-468A-98EA-B63D69D1F99D}" name="Restante" dataDxfId="21">
       <calculatedColumnFormula>B23-B10-H10-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2116,10 +2171,10 @@
 </file>
 
 <file path=xl/tables/table88.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="98" xr:uid="{7078DBBC-EA6A-4AED-9677-0F09CF55D199}" name="Table813172226303438425560657082889499" displayName="Table813172226303438425560657082889499" ref="E17:E18" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="98" xr:uid="{7078DBBC-EA6A-4AED-9677-0F09CF55D199}" name="Table813172226303438425560657082889499" displayName="Table813172226303438425560657082889499" ref="E17:E18" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{0F94546F-7898-45CB-A1C2-350CAAC13463}" name="Restante" dataDxfId="15">
+    <tableColumn id="1" xr3:uid="{0F94546F-7898-45CB-A1C2-350CAAC13463}" name="Restante" dataDxfId="18">
       <calculatedColumnFormula>B23-B10-H10-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2183,10 +2238,10 @@
 </file>
 
 <file path=xl/tables/table93.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="103" xr:uid="{D51F89B1-71F9-4429-BEFD-E895E05814BA}" name="Table813172226303438425560657082889499104" displayName="Table813172226303438425560657082889499104" ref="E17:E18" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="103" xr:uid="{D51F89B1-71F9-4429-BEFD-E895E05814BA}" name="Table813172226303438425560657082889499104" displayName="Table813172226303438425560657082889499104" ref="E17:E18" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{2D06AE74-1328-4E8B-B2E7-CA17A939DF7F}" name="Restante" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{2D06AE74-1328-4E8B-B2E7-CA17A939DF7F}" name="Restante" dataDxfId="15">
       <calculatedColumnFormula>B23-B10-H10-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2206,6 +2261,19 @@
 </file>
 
 <file path=xl/tables/table95.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="122" xr:uid="{AC0EB147-1045-4124-B23F-FB6409C6E019}" name="Table83123" displayName="Table83123" ref="G18:H20" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="G18:H20" xr:uid="{3DCA5A08-6AFF-4709-A57E-1CA655637526}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{1A1F6F3B-AAE9-46E7-9D69-F4146643520F}" name="Monto Pedido"/>
+    <tableColumn id="2" xr3:uid="{417805EC-527D-4AB6-984D-2AD532C6FC14}" name="Monto a pagar (Aprox)">
+      <calculatedColumnFormula>(G19*H18)/G18</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table96.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="72" xr:uid="{30ED15C5-06DC-4E44-B521-5DE98839EFD3}" name="Table16101419232731353952576267585919610173" displayName="Table16101419232731353952576267585919610173" ref="A2:B10" totalsRowShown="0">
   <autoFilter ref="A2:B10" xr:uid="{118E6C9A-65CE-41B2-9CDA-E2E803A2ACA4}"/>
   <tableColumns count="2">
@@ -2216,7 +2284,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table96.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table97.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="73" xr:uid="{B70A5B4A-0D4E-46BB-A3D7-76A6C2CFEC15}" name="Table271115202428323640535863688086929710274" displayName="Table271115202428323640535863688086929710274" ref="G2:H10" totalsRowShown="0">
   <autoFilter ref="G2:H10" xr:uid="{55D0E6FB-2E76-4927-9D34-9CAA769EF7F7}"/>
   <tableColumns count="2">
@@ -2227,7 +2295,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table97.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table98.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="74" xr:uid="{FFC5D93F-D0F0-439A-BC2B-0FCF618E09DB}" name="Table71216212529333741545964698187939810375" displayName="Table71216212529333741545964698187939810375" ref="A17:B23" totalsRowShown="0">
   <autoFilter ref="A17:B23" xr:uid="{5ACFFE3C-8C54-4A57-BCD6-735E5CE8DEA7}"/>
   <tableColumns count="2">
@@ -2238,26 +2306,15 @@
 </table>
 </file>
 
-<file path=xl/tables/table98.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="75" xr:uid="{385F9B9B-E896-4352-A1BA-C6D5B3B94CBD}" name="Table81317222630343842556065708288949910476" displayName="Table81317222630343842556065708288949910476" ref="E17:E18" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<file path=xl/tables/table99.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="75" xr:uid="{385F9B9B-E896-4352-A1BA-C6D5B3B94CBD}" name="Table81317222630343842556065708288949910476" displayName="Table81317222630343842556065708288949910476" ref="E17:E18" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="E17:E18" xr:uid="{8665EA2E-65C6-43BA-9A71-4634D14F02DB}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{0266BF34-9ADC-4818-9E88-FEA6FD539BF6}" name="Restante" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{0266BF34-9ADC-4818-9E88-FEA6FD539BF6}" name="Restante" dataDxfId="12">
       <calculatedColumnFormula>B23-B10-H10-E9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table99.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="89" xr:uid="{CB35E77C-BB8D-4BF0-A025-005D8F6CD22E}" name="Table434546474849515661667183899510010590" displayName="Table434546474849515661667183899510010590" ref="D2:E9" totalsRowShown="0">
-  <autoFilter ref="D2:E9" xr:uid="{35909676-23EE-45B1-96DF-AD227C9C3285}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{38930260-C22E-447F-BC3C-5F385FDA2E16}" name="Concepto"/>
-    <tableColumn id="2" xr3:uid="{88ACDE1C-DE29-4B11-8592-5C39F1030437}" name="Monto"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -2571,14 +2628,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="E1" s="17" t="s">
+      <c r="B1" s="17"/>
+      <c r="E1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="17"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2682,10 +2739,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="17"/>
+      <c r="B13" s="18"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2785,18 +2842,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="D1" s="17" t="s">
+      <c r="B1" s="17"/>
+      <c r="D1" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="G1" s="17" t="s">
+      <c r="E1" s="18"/>
+      <c r="G1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="17"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2934,10 +2991,10 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="17"/>
+      <c r="B16" s="18"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3022,18 +3079,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="D1" s="17" t="s">
+      <c r="B1" s="17"/>
+      <c r="D1" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="G1" s="17" t="s">
+      <c r="E1" s="18"/>
+      <c r="G1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="17"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3156,10 +3213,10 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="17"/>
+      <c r="B16" s="18"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3236,18 +3293,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="D1" s="17" t="s">
+      <c r="B1" s="17"/>
+      <c r="D1" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="G1" s="17" t="s">
+      <c r="E1" s="18"/>
+      <c r="G1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="17"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3388,10 +3445,10 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="17"/>
+      <c r="B16" s="18"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3468,18 +3525,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="D1" s="17" t="s">
+      <c r="B1" s="17"/>
+      <c r="D1" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="G1" s="17" t="s">
+      <c r="E1" s="18"/>
+      <c r="G1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="17"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3599,10 +3656,10 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="17"/>
+      <c r="B16" s="18"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3667,8 +3724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D62384EF-D9B2-497E-AA08-6F8BC70A67AB}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15:I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3680,18 +3737,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="D1" s="17" t="s">
+      <c r="B1" s="17"/>
+      <c r="D1" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="G1" s="17" t="s">
+      <c r="E1" s="18"/>
+      <c r="G1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="17"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3796,16 +3853,16 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H15" s="17" t="s">
+      <c r="H15" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="I15" s="17"/>
+      <c r="I15" s="18"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="17"/>
+      <c r="B16" s="18"/>
       <c r="H16" s="13" t="s">
         <v>108</v>
       </c>
@@ -3895,18 +3952,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="D1" s="17" t="s">
+      <c r="B1" s="17"/>
+      <c r="D1" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="G1" s="17" t="s">
+      <c r="E1" s="18"/>
+      <c r="G1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="17"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -4032,14 +4089,14 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="17"/>
+      <c r="B16" s="18"/>
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
     </row>
@@ -4099,7 +4156,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4111,18 +4168,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="D1" s="17" t="s">
+      <c r="B1" s="17"/>
+      <c r="D1" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="G1" s="17" t="s">
+      <c r="E1" s="18"/>
+      <c r="G1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="17"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -4251,14 +4308,14 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="17"/>
+      <c r="B16" s="18"/>
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
     </row>
@@ -4338,18 +4395,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="D1" s="17" t="s">
+      <c r="B1" s="17"/>
+      <c r="D1" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="G1" s="17" t="s">
+      <c r="E1" s="18"/>
+      <c r="G1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="17"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -4376,7 +4433,7 @@
         <v>28</v>
       </c>
       <c r="B3">
-        <v>6000</v>
+        <v>6100</v>
       </c>
       <c r="D3" t="s">
         <v>113</v>
@@ -4403,7 +4460,7 @@
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="6">
         <v>4800</v>
       </c>
       <c r="G5" t="s">
@@ -4415,7 +4472,7 @@
         <v>125</v>
       </c>
       <c r="B6">
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="G6" t="s">
         <v>15</v>
@@ -4450,6 +4507,12 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9">
+        <v>350</v>
+      </c>
       <c r="D9" t="s">
         <v>5</v>
       </c>
@@ -4467,7 +4530,7 @@
       </c>
       <c r="B10">
         <f>SUM(B3:B9)</f>
-        <v>15074</v>
+        <v>15424</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
@@ -4478,14 +4541,14 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="17"/>
+      <c r="B16" s="18"/>
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
     </row>
@@ -4509,7 +4572,7 @@
       </c>
       <c r="E18" s="13">
         <f>B23-B10-H10-E9</f>
-        <v>2026</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -4517,7 +4580,7 @@
         <v>7</v>
       </c>
       <c r="B19">
-        <v>6600</v>
+        <v>6900</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -4526,7 +4589,7 @@
       </c>
       <c r="B23">
         <f>SUM(B18:B22)</f>
-        <v>21600</v>
+        <v>21900</v>
       </c>
     </row>
   </sheetData>
@@ -4553,6 +4616,242 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17:H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="26.85546875" customWidth="1"/>
+    <col min="4" max="5" width="18.7109375" customWidth="1"/>
+    <col min="7" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="D1" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="18"/>
+      <c r="G1" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="18"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3">
+        <v>1500</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>2650</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>8300</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <f>SUM(E3:E8)</f>
+        <v>1500</v>
+      </c>
+      <c r="G9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <f>SUM(B3:B9)</f>
+        <v>10950</v>
+      </c>
+      <c r="G10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <f>SUM(H3:H9)</f>
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="18"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="H17" s="18"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>15000</v>
+      </c>
+      <c r="E18" s="13">
+        <f>B23-B10-H10-E9</f>
+        <v>1950</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19">
+        <v>5900</v>
+      </c>
+      <c r="G19">
+        <v>6900</v>
+      </c>
+      <c r="H19">
+        <v>8300</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>5900</v>
+      </c>
+      <c r="H20">
+        <f>(G20*H19)/G19</f>
+        <v>7097.101449275362</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <f>SUM(B18:B22)</f>
+        <v>20900</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="A16:B16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="6">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDEB9995-7AFA-4020-994D-E08589C59BFF}">
+  <dimension ref="A1:I23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -4565,18 +4864,731 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="D1" s="17" t="s">
+      <c r="B1" s="17"/>
+      <c r="D1" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="G1" s="17" t="s">
+      <c r="E1" s="18"/>
+      <c r="G1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="17"/>
+      <c r="H1" s="18"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3">
+        <v>1500</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>2650</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>7100</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <f>SUM(E3:E8)</f>
+        <v>1500</v>
+      </c>
+      <c r="G9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <f>SUM(B3:B9)</f>
+        <v>9750</v>
+      </c>
+      <c r="G10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <f>SUM(H3:H9)</f>
+        <v>4900</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="18"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="H17" s="18"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>15000</v>
+      </c>
+      <c r="E18" s="15">
+        <f>B23-B10-H10-E9</f>
+        <v>2050</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19">
+        <v>3200</v>
+      </c>
+      <c r="G19">
+        <v>5900</v>
+      </c>
+      <c r="H19">
+        <v>7100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>3200</v>
+      </c>
+      <c r="H20">
+        <f>(G20*H19)/G19</f>
+        <v>3850.8474576271187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <f>SUM(B18:B22)</f>
+        <v>18200</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="A16:B16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="6">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B619FC8B-C472-4B3F-A5C2-E94C99B67E8C}">
+  <dimension ref="A1:F23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="26.85546875" customWidth="1"/>
+    <col min="5" max="6" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="E1" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="18"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <f>2100+360</f>
+        <v>2460</v>
+      </c>
+      <c r="C3">
+        <f>1145+700</f>
+        <v>1845</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>3670</v>
+      </c>
+      <c r="C4" s="4">
+        <v>3670</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>1100</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1445</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="4">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6">
+        <v>1000</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7">
+        <v>400</v>
+      </c>
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="4">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8">
+        <v>700</v>
+      </c>
+      <c r="C8" s="4">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>1175</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1175</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <f>SUM(F3:F8)</f>
+        <v>3970</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10">
+        <v>1000</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <f>SUM(B3:B10)</f>
+        <v>11505</v>
+      </c>
+      <c r="C12">
+        <f>SUM(C3:C10)</f>
+        <v>10915</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="18"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>15000</v>
+      </c>
+      <c r="F18" s="1">
+        <f>B23-C12-F9</f>
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <f>SUM(B18:B22)</f>
+        <v>16000</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A16:B16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="4">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFECC3C-B62E-49F5-A68F-6241052BDF14}">
+  <dimension ref="A1:I23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="26.85546875" customWidth="1"/>
+    <col min="4" max="5" width="18.7109375" customWidth="1"/>
+    <col min="7" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="D1" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="18"/>
+      <c r="G1" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="18"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3">
+        <v>1500</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>2650</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>3800</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6">
+        <v>1550</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <f>SUM(E3:E8)</f>
+        <v>1500</v>
+      </c>
+      <c r="G9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <f>SUM(B3:B9)</f>
+        <v>8000</v>
+      </c>
+      <c r="G10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <f>SUM(H3:H9)</f>
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="18"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="H17" s="18"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>15000</v>
+      </c>
+      <c r="E18" s="15">
+        <f>B23-B10-H10-E9</f>
+        <v>2000</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>5900</v>
+      </c>
+      <c r="H19">
+        <v>7100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>3200</v>
+      </c>
+      <c r="H20">
+        <f>(G20*H19)/G19</f>
+        <v>3850.8474576271187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <f>SUM(B18:B22)</f>
+        <v>15000</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="A16:B16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="6">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7896DF-CDEF-471C-A59C-7B910269B67F}">
+  <dimension ref="A1:I23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="26.85546875" customWidth="1"/>
+    <col min="4" max="5" width="18.7109375" customWidth="1"/>
+    <col min="7" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="D1" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="18"/>
+      <c r="G1" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -4612,7 +5624,7 @@
         <v>11</v>
       </c>
       <c r="H3">
-        <v>3500</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -4625,13 +5637,16 @@
       <c r="G4" t="s">
         <v>13</v>
       </c>
+      <c r="H4">
+        <v>300</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="B5">
-        <v>7500</v>
+        <v>3950</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
@@ -4642,7 +5657,7 @@
         <v>15</v>
       </c>
       <c r="H6">
-        <v>2000</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -4676,27 +5691,27 @@
       </c>
       <c r="B10">
         <f>SUM(B3:B9)</f>
-        <v>10150</v>
+        <v>6600</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
       </c>
       <c r="H10">
         <f>SUM(H3:H9)</f>
-        <v>6500</v>
+        <v>4900</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
+      <c r="B16" s="18"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -4705,7 +5720,7 @@
       <c r="B17" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="15" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4716,17 +5731,9 @@
       <c r="B18">
         <v>15000</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="15">
         <f>B23-B10-H10-E9</f>
-        <v>2050</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19">
-        <v>5200</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -4735,7 +5742,7 @@
       </c>
       <c r="B23">
         <f>SUM(B18:B22)</f>
-        <v>20200</v>
+        <v>15000</v>
       </c>
     </row>
   </sheetData>
@@ -4757,8 +5764,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDEB9995-7AFA-4020-994D-E08589C59BFF}">
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B65F810-9C84-4DE0-9AC5-AAEA1E957A65}">
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4774,18 +5781,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="D1" s="17" t="s">
+      <c r="B1" s="17"/>
+      <c r="D1" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="G1" s="17" t="s">
+      <c r="E1" s="18"/>
+      <c r="G1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="17"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -4808,17 +5815,11 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E3">
-        <v>1500</v>
-      </c>
       <c r="G3" t="s">
         <v>11</v>
       </c>
       <c r="H3">
-        <v>1500</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -4832,15 +5833,15 @@
         <v>13</v>
       </c>
       <c r="H4">
-        <v>400</v>
+        <v>300</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="B5">
-        <v>6000</v>
+        <v>4950</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
@@ -4851,7 +5852,7 @@
         <v>15</v>
       </c>
       <c r="H6">
-        <v>2000</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -4873,7 +5874,7 @@
       </c>
       <c r="E9">
         <f>SUM(E3:E8)</f>
-        <v>1500</v>
+        <v>0</v>
       </c>
       <c r="G9" t="s">
         <v>96</v>
@@ -4885,25 +5886,25 @@
       </c>
       <c r="B10">
         <f>SUM(B3:B9)</f>
-        <v>8650</v>
+        <v>7600</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
       </c>
       <c r="H10">
         <f>SUM(H3:H9)</f>
-        <v>4900</v>
+        <v>5400</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="17"/>
+      <c r="B16" s="18"/>
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
     </row>
@@ -4927,15 +5928,7 @@
       </c>
       <c r="E18" s="15">
         <f>B23-B10-H10-E9</f>
-        <v>2050</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19">
-        <v>2100</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -4944,7 +5937,7 @@
       </c>
       <c r="B23">
         <f>SUM(B18:B22)</f>
-        <v>17100</v>
+        <v>15000</v>
       </c>
     </row>
   </sheetData>
@@ -4966,856 +5959,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B619FC8B-C472-4B3F-A5C2-E94C99B67E8C}">
-  <dimension ref="A1:F23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="26.85546875" customWidth="1"/>
-    <col min="5" max="6" width="21" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="E1" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="17"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <f>2100+360</f>
-        <v>2460</v>
-      </c>
-      <c r="C3">
-        <f>1145+700</f>
-        <v>1845</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="4">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>3670</v>
-      </c>
-      <c r="C4" s="4">
-        <v>3670</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>1100</v>
-      </c>
-      <c r="C5" s="4">
-        <v>1445</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="4">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6">
-        <v>1000</v>
-      </c>
-      <c r="C6" s="4">
-        <v>1000</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="4">
-        <v>1350</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7">
-        <v>400</v>
-      </c>
-      <c r="E7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="4">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8">
-        <v>700</v>
-      </c>
-      <c r="C8" s="4">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>1175</v>
-      </c>
-      <c r="C9" s="4">
-        <v>1175</v>
-      </c>
-      <c r="E9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9">
-        <f>SUM(F3:F8)</f>
-        <v>3970</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10">
-        <v>1000</v>
-      </c>
-      <c r="C10" s="4">
-        <v>1080</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12">
-        <f>SUM(B3:B10)</f>
-        <v>11505</v>
-      </c>
-      <c r="C12">
-        <f>SUM(C3:C10)</f>
-        <v>10915</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="17"/>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18">
-        <v>15000</v>
-      </c>
-      <c r="F18" s="1">
-        <f>B23-C12-F9</f>
-        <v>1115</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23">
-        <f>SUM(B18:B22)</f>
-        <v>16000</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A16:B16"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="4">
-    <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
-    <tablePart r:id="rId4"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFECC3C-B62E-49F5-A68F-6241052BDF14}">
-  <dimension ref="A1:I23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="26.85546875" customWidth="1"/>
-    <col min="4" max="5" width="18.7109375" customWidth="1"/>
-    <col min="7" max="8" width="21" customWidth="1"/>
-    <col min="9" max="9" width="28" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="D1" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="17"/>
-      <c r="G1" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="17"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E3">
-        <v>1500</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>2650</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>3000</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>127</v>
-      </c>
-      <c r="B6">
-        <v>450</v>
-      </c>
-      <c r="G6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6">
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9">
-        <f>SUM(E3:E8)</f>
-        <v>1500</v>
-      </c>
-      <c r="G9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10">
-        <f>SUM(B3:B9)</f>
-        <v>6100</v>
-      </c>
-      <c r="G10" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10">
-        <f>SUM(H3:H9)</f>
-        <v>5400</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="17"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18">
-        <v>15000</v>
-      </c>
-      <c r="E18" s="15">
-        <f>B23-B10-H10-E9</f>
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23">
-        <f>SUM(B18:B22)</f>
-        <v>15000</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="A16:B16"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="5">
-    <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
-    <tablePart r:id="rId4"/>
-    <tablePart r:id="rId5"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7896DF-CDEF-471C-A59C-7B910269B67F}">
-  <dimension ref="A1:I23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="26.85546875" customWidth="1"/>
-    <col min="4" max="5" width="18.7109375" customWidth="1"/>
-    <col min="7" max="8" width="21" customWidth="1"/>
-    <col min="9" max="9" width="28" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="D1" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="17"/>
-      <c r="G1" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="17"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E3">
-        <v>1500</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>2650</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B5">
-        <v>3950</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6">
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9">
-        <f>SUM(E3:E8)</f>
-        <v>1500</v>
-      </c>
-      <c r="G9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10">
-        <f>SUM(B3:B9)</f>
-        <v>6600</v>
-      </c>
-      <c r="G10" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10">
-        <f>SUM(H3:H9)</f>
-        <v>4900</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="17"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18">
-        <v>15000</v>
-      </c>
-      <c r="E18" s="15">
-        <f>B23-B10-H10-E9</f>
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23">
-        <f>SUM(B18:B22)</f>
-        <v>15000</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="A16:B16"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="5">
-    <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
-    <tablePart r:id="rId4"/>
-    <tablePart r:id="rId5"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B65F810-9C84-4DE0-9AC5-AAEA1E957A65}">
-  <dimension ref="A1:I23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="26.85546875" customWidth="1"/>
-    <col min="4" max="5" width="18.7109375" customWidth="1"/>
-    <col min="7" max="8" width="21" customWidth="1"/>
-    <col min="9" max="9" width="28" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="D1" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="17"/>
-      <c r="G1" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="17"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>2650</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B5">
-        <v>4950</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6">
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9">
-        <f>SUM(E3:E8)</f>
-        <v>0</v>
-      </c>
-      <c r="G9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10">
-        <f>SUM(B3:B9)</f>
-        <v>7600</v>
-      </c>
-      <c r="G10" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10">
-        <f>SUM(H3:H9)</f>
-        <v>5400</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="17"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18">
-        <v>15000</v>
-      </c>
-      <c r="E18" s="15">
-        <f>B23-B10-H10-E9</f>
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23">
-        <f>SUM(B18:B22)</f>
-        <v>15000</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="A16:B16"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="5">
-    <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
-    <tablePart r:id="rId4"/>
-    <tablePart r:id="rId5"/>
-  </tableParts>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C91EC96-E704-492F-899B-E65E27E820DF}">
   <dimension ref="A1:J13"/>
@@ -5831,10 +5974,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="16"/>
+      <c r="B1" s="17"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -6920,18 +7063,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="D1" s="17" t="s">
+      <c r="B1" s="17"/>
+      <c r="D1" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="G1" s="17" t="s">
+      <c r="E1" s="18"/>
+      <c r="G1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="17"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -7057,16 +7200,16 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="H16" s="17"/>
+      <c r="H16" s="18"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="17"/>
+      <c r="B17" s="18"/>
       <c r="E17" s="2" t="s">
         <v>12</v>
       </c>
@@ -7183,18 +7326,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="D1" s="17" t="s">
+      <c r="B1" s="17"/>
+      <c r="D1" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="G1" s="17" t="s">
+      <c r="E1" s="18"/>
+      <c r="G1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="17"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -7329,14 +7472,14 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="G16" s="17" t="s">
+      <c r="B16" s="18"/>
+      <c r="G16" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="H16" s="17"/>
+      <c r="H16" s="18"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -7443,18 +7586,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="D1" s="17" t="s">
+      <c r="B1" s="17"/>
+      <c r="D1" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="G1" s="17" t="s">
+      <c r="E1" s="18"/>
+      <c r="G1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="17"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -7578,10 +7721,10 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="17"/>
+      <c r="B16" s="18"/>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -7666,18 +7809,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="D1" s="17" t="s">
+      <c r="B1" s="17"/>
+      <c r="D1" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="G1" s="17" t="s">
+      <c r="E1" s="18"/>
+      <c r="G1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="17"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -7815,10 +7958,10 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="17"/>
+      <c r="B16" s="18"/>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -7887,18 +8030,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="D1" s="17" t="s">
+      <c r="B1" s="17"/>
+      <c r="D1" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="G1" s="17" t="s">
+      <c r="E1" s="18"/>
+      <c r="G1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="17"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -8042,10 +8185,10 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="17"/>
+      <c r="B16" s="18"/>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -8122,18 +8265,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="D1" s="17" t="s">
+      <c r="B1" s="17"/>
+      <c r="D1" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="G1" s="17" t="s">
+      <c r="E1" s="18"/>
+      <c r="G1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="17"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -8253,10 +8396,10 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="17"/>
+      <c r="B16" s="18"/>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -8327,18 +8470,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="D1" s="17" t="s">
+      <c r="B1" s="17"/>
+      <c r="D1" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="G1" s="17" t="s">
+      <c r="E1" s="18"/>
+      <c r="G1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="17"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -8477,10 +8620,10 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G14" s="17" t="s">
+      <c r="G14" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="H14" s="17"/>
+      <c r="H14" s="18"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G15" t="s">
@@ -8494,10 +8637,10 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="17"/>
+      <c r="B16" s="18"/>
       <c r="G16" s="6" t="s">
         <v>6</v>
       </c>
@@ -8572,10 +8715,10 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="E21" s="17"/>
+      <c r="E21" s="18"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D22" t="s">

</xml_diff>